<commit_message>
fonts from loc db
</commit_message>
<xml_diff>
--- a/fonts/localization.xlsx
+++ b/fonts/localization.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\fonts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CADB8F-5161-4E9C-8B48-557687DF21A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D39F6E-010A-4BE7-8AFF-9BD5FEF81AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="6" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="19200" windowHeight="10073" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
-    <sheet name="Font" sheetId="6" r:id="rId1"/>
+    <sheet name="Fonts" sheetId="6" r:id="rId1"/>
     <sheet name="Colors" sheetId="7" r:id="rId2"/>
     <sheet name="Page" sheetId="1" r:id="rId3"/>
     <sheet name="Stage" sheetId="4" r:id="rId4"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="714">
   <si>
     <t>key</t>
   </si>
@@ -2086,18 +2086,9 @@
     <t>TradeGothicLTStd-BdCn20.otf</t>
   </si>
   <si>
-    <t>calendar.dayofweek</t>
-  </si>
-  <si>
     <t>alt-en</t>
   </si>
   <si>
-    <t>day.time</t>
-  </si>
-  <si>
-    <t>day.form.label</t>
-  </si>
-  <si>
     <t>consolab.ttf</t>
   </si>
   <si>
@@ -2201,6 +2192,9 @@
   </si>
   <si>
     <t>#eecbef</t>
+  </si>
+  <si>
+    <t>calendar.day-of-week</t>
   </si>
 </sst>
 </file>
@@ -2288,8 +2282,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}" name="Table1" displayName="Table1" ref="A1:J22" totalsRowShown="0">
-  <autoFilter ref="A1:J22" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}" name="Table1" displayName="Table1" ref="A1:J20" totalsRowShown="0">
+  <autoFilter ref="A1:J20" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4614A9ED-E890-4F3B-BD19-53C40876125F}" name="key"/>
     <tableColumn id="2" xr3:uid="{8969FEC0-AADF-46CE-8C23-D03ADE795753}" name="en"/>
@@ -2712,15 +2706,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4B28FF-857C-4B73-BD2F-84CA03D2F2FC}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="16.703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.9375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.87890625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.87890625" customWidth="1"/>
     <col min="9" max="9" width="11.9375" bestFit="1" customWidth="1"/>
@@ -2734,7 +2728,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2766,13 +2760,13 @@
         <v>669</v>
       </c>
       <c r="C2" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="I2" t="s">
         <v>669</v>
       </c>
       <c r="J2" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.5">
@@ -2783,13 +2777,13 @@
         <v>670</v>
       </c>
       <c r="C3" t="s">
+        <v>679</v>
+      </c>
+      <c r="I3" t="s">
         <v>682</v>
       </c>
-      <c r="I3" t="s">
-        <v>685</v>
-      </c>
       <c r="J3" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.5">
@@ -2800,13 +2794,13 @@
         <v>671</v>
       </c>
       <c r="C4" t="s">
+        <v>679</v>
+      </c>
+      <c r="I4" t="s">
         <v>682</v>
       </c>
-      <c r="I4" t="s">
-        <v>685</v>
-      </c>
       <c r="J4" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.5">
@@ -2817,13 +2811,13 @@
         <v>671</v>
       </c>
       <c r="C5" t="s">
+        <v>679</v>
+      </c>
+      <c r="I5" t="s">
         <v>682</v>
       </c>
-      <c r="I5" t="s">
-        <v>685</v>
-      </c>
       <c r="J5" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.5">
@@ -2851,262 +2845,234 @@
         <v>672</v>
       </c>
       <c r="C7" t="s">
+        <v>680</v>
+      </c>
+      <c r="I7" t="s">
         <v>683</v>
       </c>
-      <c r="I7" t="s">
-        <v>686</v>
-      </c>
       <c r="J7" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
+        <v>657</v>
+      </c>
+      <c r="B8" t="s">
+        <v>673</v>
+      </c>
+      <c r="C8" t="s">
         <v>679</v>
       </c>
-      <c r="C8" t="s">
-        <v>682</v>
-      </c>
       <c r="I8" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="J8" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>680</v>
+        <v>658</v>
+      </c>
+      <c r="B9" t="s">
+        <v>669</v>
       </c>
       <c r="C9" t="s">
-        <v>682</v>
+        <v>669</v>
       </c>
       <c r="I9" t="s">
-        <v>686</v>
+        <v>669</v>
       </c>
       <c r="J9" t="s">
-        <v>682</v>
+        <v>669</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B10" t="s">
         <v>673</v>
       </c>
       <c r="C10" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="I10" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="J10" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B11" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
       <c r="C11" t="s">
-        <v>669</v>
+        <v>681</v>
       </c>
       <c r="I11" t="s">
-        <v>669</v>
+        <v>684</v>
       </c>
       <c r="J11" t="s">
-        <v>669</v>
+        <v>681</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="B12" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="C12" t="s">
+        <v>679</v>
+      </c>
+      <c r="I12" t="s">
         <v>682</v>
       </c>
-      <c r="I12" t="s">
-        <v>686</v>
-      </c>
       <c r="J12" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="B13" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C13" t="s">
+        <v>681</v>
+      </c>
+      <c r="I13" t="s">
         <v>684</v>
       </c>
-      <c r="I13" t="s">
-        <v>687</v>
-      </c>
       <c r="J13" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="B14" t="s">
         <v>670</v>
       </c>
       <c r="C14" t="s">
+        <v>679</v>
+      </c>
+      <c r="I14" t="s">
         <v>682</v>
       </c>
-      <c r="I14" t="s">
-        <v>685</v>
-      </c>
       <c r="J14" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="B15" t="s">
         <v>675</v>
       </c>
       <c r="C15" t="s">
+        <v>681</v>
+      </c>
+      <c r="I15" t="s">
         <v>684</v>
       </c>
-      <c r="I15" t="s">
-        <v>687</v>
-      </c>
       <c r="J15" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="B16" t="s">
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="C16" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I16" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="J16" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="B17" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C17" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="I17" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="J17" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="B18" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="C18" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="I18" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="J18" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="B19" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="C19" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I19" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="J19" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>667</v>
+        <v>713</v>
       </c>
       <c r="B20" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C20" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="I20" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="J20" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A21" t="s">
-        <v>668</v>
-      </c>
-      <c r="B21" t="s">
-        <v>676</v>
-      </c>
-      <c r="C21" t="s">
-        <v>684</v>
-      </c>
-      <c r="I21" t="s">
-        <v>687</v>
-      </c>
-      <c r="J21" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A22" t="s">
-        <v>677</v>
-      </c>
-      <c r="B22" t="s">
-        <v>672</v>
-      </c>
-      <c r="C22" t="s">
-        <v>683</v>
-      </c>
-      <c r="I22" t="s">
-        <v>686</v>
-      </c>
-      <c r="J22" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
   </sheetData>
@@ -3159,66 +3125,66 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="B2" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="B3" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="B4" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="B5" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B6" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B7" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="B8" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="B9" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
     </row>
   </sheetData>
@@ -3600,7 +3566,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -3632,16 +3598,16 @@
         <v>639</v>
       </c>
       <c r="B3" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="C3" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
@@ -3650,7 +3616,7 @@
         <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
@@ -3661,7 +3627,7 @@
         <v>31</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
@@ -3672,7 +3638,7 @@
         <v>32</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
   </sheetData>
@@ -3704,7 +3670,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3736,28 +3702,28 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
+        <v>686</v>
+      </c>
+      <c r="D2" t="s">
+        <v>687</v>
+      </c>
+      <c r="E2" t="s">
+        <v>687</v>
+      </c>
+      <c r="F2" t="s">
+        <v>687</v>
+      </c>
+      <c r="G2" t="s">
+        <v>688</v>
+      </c>
+      <c r="H2" t="s">
         <v>689</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>690</v>
       </c>
-      <c r="E2" t="s">
-        <v>690</v>
-      </c>
-      <c r="F2" t="s">
-        <v>690</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>691</v>
-      </c>
-      <c r="H2" t="s">
-        <v>692</v>
-      </c>
-      <c r="I2" t="s">
-        <v>693</v>
-      </c>
-      <c r="J2" t="s">
-        <v>694</v>
       </c>
     </row>
   </sheetData>
@@ -3772,7 +3738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5C7B9E-E03D-420F-8955-42B4860CC822}">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>

</xml_diff>

<commit_message>
farsi fixes (rtl calendar + spelling)
</commit_message>
<xml_diff>
--- a/fonts/localization.xlsx
+++ b/fonts/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\fonts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A998DDBB-8042-4C03-9A31-ADC40A5EFA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF24BB4-0B9F-49B6-A292-48FB5F5F6AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="-9973" yWindow="4527" windowWidth="19200" windowHeight="10073" activeTab="6" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonts" sheetId="6" r:id="rId1"/>
@@ -370,9 +370,6 @@
     <t>アルゼンチン</t>
   </si>
   <si>
-    <t>وابسته به آرژانتین</t>
-  </si>
-  <si>
     <t>England</t>
   </si>
   <si>
@@ -448,9 +445,6 @@
     <t>ポルトガル</t>
   </si>
   <si>
-    <t>کشور پرتغال</t>
-  </si>
-  <si>
     <t>Mexico</t>
   </si>
   <si>
@@ -550,9 +544,6 @@
     <t>ウルグアイ</t>
   </si>
   <si>
-    <t>اروغای</t>
-  </si>
-  <si>
     <t>Switzerland</t>
   </si>
   <si>
@@ -748,9 +739,6 @@
     <t>モロッコ</t>
   </si>
   <si>
-    <t>مراکشی</t>
-  </si>
-  <si>
     <t>Serbia</t>
   </si>
   <si>
@@ -2195,6 +2183,18 @@
   </si>
   <si>
     <t>calendar.day-of-week</t>
+  </si>
+  <si>
+    <t>پرتغال</t>
+  </si>
+  <si>
+    <t>اروگوئه</t>
+  </si>
+  <si>
+    <t>آرژانتین</t>
+  </si>
+  <si>
+    <t>مراکش</t>
   </si>
 </sst>
 </file>
@@ -2708,7 +2708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4B28FF-857C-4B73-BD2F-84CA03D2F2FC}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -2729,7 +2729,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2755,325 +2755,325 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="B2" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C2" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="I2" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="J2" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="B3" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C3" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="I3" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="J3" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B4" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C4" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="I4" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="J4" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B5" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="C5" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="I5" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="J5" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="B6" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C6" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="I6" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="J6" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="B7" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="C7" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="I7" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="J7" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="B8" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="C8" t="s">
+        <v>675</v>
+      </c>
+      <c r="I8" t="s">
         <v>679</v>
       </c>
-      <c r="I8" t="s">
-        <v>683</v>
-      </c>
       <c r="J8" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="B9" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="C9" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="I9" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="J9" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B10" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="C10" t="s">
+        <v>675</v>
+      </c>
+      <c r="I10" t="s">
         <v>679</v>
       </c>
-      <c r="I10" t="s">
-        <v>683</v>
-      </c>
       <c r="J10" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="B11" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C11" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="I11" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="J11" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="B12" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C12" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="I12" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="J12" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B13" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C13" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="I13" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="J13" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="B14" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C14" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="I14" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="J14" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="B15" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C15" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="I15" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="J15" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B16" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="C16" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="I16" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="J16" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B17" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="C17" t="s">
+        <v>675</v>
+      </c>
+      <c r="I17" t="s">
         <v>679</v>
       </c>
-      <c r="I17" t="s">
-        <v>683</v>
-      </c>
       <c r="J17" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="B18" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="C18" t="s">
+        <v>675</v>
+      </c>
+      <c r="I18" t="s">
         <v>679</v>
       </c>
-      <c r="I18" t="s">
-        <v>683</v>
-      </c>
       <c r="J18" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="B19" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="C19" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="I19" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="J19" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="B20" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="C20" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="I20" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="J20" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
   </sheetData>
@@ -3126,66 +3126,66 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="B2" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="B3" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="B4" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="B5" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="B6" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="B7" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="B8" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="B9" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
   </sheetData>
@@ -3240,7 +3240,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -3269,7 +3269,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
@@ -3277,7 +3277,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -3372,7 +3372,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -3401,7 +3401,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
@@ -3430,7 +3430,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>
@@ -3459,7 +3459,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B6" t="s">
         <v>65</v>
@@ -3488,7 +3488,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B7" t="s">
         <v>73</v>
@@ -3567,7 +3567,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -3596,19 +3596,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="B3" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="C3" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
@@ -3617,29 +3617,29 @@
         <v>30</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
     </row>
   </sheetData>
@@ -3671,7 +3671,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3697,34 +3697,34 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
       <c r="C2" t="s">
+        <v>682</v>
+      </c>
+      <c r="D2" t="s">
+        <v>683</v>
+      </c>
+      <c r="E2" t="s">
+        <v>683</v>
+      </c>
+      <c r="F2" t="s">
+        <v>683</v>
+      </c>
+      <c r="G2" t="s">
+        <v>684</v>
+      </c>
+      <c r="H2" t="s">
+        <v>685</v>
+      </c>
+      <c r="I2" t="s">
         <v>686</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J2" t="s">
         <v>687</v>
-      </c>
-      <c r="E2" t="s">
-        <v>687</v>
-      </c>
-      <c r="F2" t="s">
-        <v>687</v>
-      </c>
-      <c r="G2" t="s">
-        <v>688</v>
-      </c>
-      <c r="H2" t="s">
-        <v>689</v>
-      </c>
-      <c r="I2" t="s">
-        <v>690</v>
-      </c>
-      <c r="J2" t="s">
-        <v>691</v>
       </c>
     </row>
   </sheetData>
@@ -3739,9 +3739,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5C7B9E-E03D-420F-8955-42B4860CC822}">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="5.8203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.52734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.9375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.29296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.29296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.87890625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.29296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
@@ -3774,7 +3789,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B2" t="s">
         <v>78</v>
@@ -3803,7 +3818,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B3" t="s">
         <v>86</v>
@@ -3832,7 +3847,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B4" t="s">
         <v>94</v>
@@ -3861,7 +3876,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B5" t="s">
         <v>100</v>
@@ -3885,2182 +3900,2182 @@
         <v>104</v>
       </c>
       <c r="I5" t="s">
-        <v>105</v>
+        <v>712</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" t="s">
         <v>106</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>107</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>108</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" t="s">
         <v>109</v>
       </c>
-      <c r="F6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>110</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>111</v>
-      </c>
-      <c r="I6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
         <v>113</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" t="s">
         <v>114</v>
       </c>
-      <c r="D7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>115</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>116</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>117</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>118</v>
-      </c>
-      <c r="I7" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" t="s">
         <v>120</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>121</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>122</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>123</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>124</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>125</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>126</v>
-      </c>
-      <c r="I8" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" t="s">
         <v>128</v>
       </c>
-      <c r="C9" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" t="s">
         <v>129</v>
       </c>
-      <c r="E9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F9" t="s">
-        <v>128</v>
-      </c>
-      <c r="G9" t="s">
-        <v>128</v>
-      </c>
-      <c r="H9" t="s">
-        <v>130</v>
-      </c>
       <c r="I9" t="s">
-        <v>131</v>
+        <v>710</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" t="s">
         <v>132</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>133</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>134</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" t="s">
         <v>135</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>136</v>
-      </c>
-      <c r="G10" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" t="s">
-        <v>137</v>
-      </c>
-      <c r="I10" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" t="s">
         <v>139</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>140</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>141</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>142</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>143</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>144</v>
-      </c>
-      <c r="H11" t="s">
-        <v>145</v>
-      </c>
-      <c r="I11" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" t="s">
         <v>147</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>148</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>149</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>150</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>151</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>152</v>
-      </c>
-      <c r="H12" t="s">
-        <v>153</v>
-      </c>
-      <c r="I12" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" t="s">
         <v>155</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>156</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>157</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>158</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>159</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>160</v>
-      </c>
-      <c r="H13" t="s">
-        <v>161</v>
-      </c>
-      <c r="I13" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="B14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I14" t="s">
-        <v>165</v>
+        <v>711</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" t="s">
+        <v>165</v>
+      </c>
+      <c r="E15" t="s">
         <v>166</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>167</v>
       </c>
-      <c r="D15" t="s">
+      <c r="G15" t="s">
         <v>168</v>
       </c>
-      <c r="E15" t="s">
+      <c r="H15" t="s">
         <v>169</v>
       </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>170</v>
-      </c>
-      <c r="G15" t="s">
-        <v>171</v>
-      </c>
-      <c r="H15" t="s">
-        <v>172</v>
-      </c>
-      <c r="I15" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" t="s">
+        <v>171</v>
+      </c>
+      <c r="E16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F16" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" t="s">
+        <v>171</v>
+      </c>
+      <c r="H16" t="s">
+        <v>173</v>
+      </c>
+      <c r="I16" t="s">
         <v>174</v>
-      </c>
-      <c r="C16" t="s">
-        <v>175</v>
-      </c>
-      <c r="D16" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" t="s">
-        <v>174</v>
-      </c>
-      <c r="F16" t="s">
-        <v>174</v>
-      </c>
-      <c r="G16" t="s">
-        <v>174</v>
-      </c>
-      <c r="H16" t="s">
-        <v>176</v>
-      </c>
-      <c r="I16" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D17" t="s">
+        <v>177</v>
+      </c>
+      <c r="E17" t="s">
         <v>178</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
         <v>179</v>
       </c>
-      <c r="D17" t="s">
+      <c r="G17" t="s">
         <v>180</v>
       </c>
-      <c r="E17" t="s">
+      <c r="H17" t="s">
         <v>181</v>
       </c>
-      <c r="F17" t="s">
+      <c r="I17" t="s">
         <v>182</v>
-      </c>
-      <c r="G17" t="s">
-        <v>183</v>
-      </c>
-      <c r="H17" t="s">
-        <v>184</v>
-      </c>
-      <c r="I17" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="B18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D18" t="s">
+        <v>183</v>
+      </c>
+      <c r="E18" t="s">
+        <v>184</v>
+      </c>
+      <c r="F18" t="s">
+        <v>185</v>
+      </c>
+      <c r="G18" t="s">
+        <v>183</v>
+      </c>
+      <c r="H18" t="s">
         <v>186</v>
       </c>
-      <c r="C18" t="s">
-        <v>186</v>
-      </c>
-      <c r="D18" t="s">
-        <v>186</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="I18" t="s">
         <v>187</v>
-      </c>
-      <c r="F18" t="s">
-        <v>188</v>
-      </c>
-      <c r="G18" t="s">
-        <v>186</v>
-      </c>
-      <c r="H18" t="s">
-        <v>189</v>
-      </c>
-      <c r="I18" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C19" t="s">
+        <v>189</v>
+      </c>
+      <c r="D19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E19" t="s">
         <v>191</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" t="s">
+        <v>188</v>
+      </c>
+      <c r="G19" t="s">
+        <v>188</v>
+      </c>
+      <c r="H19" t="s">
         <v>192</v>
       </c>
-      <c r="D19" t="s">
+      <c r="I19" t="s">
         <v>193</v>
-      </c>
-      <c r="E19" t="s">
-        <v>194</v>
-      </c>
-      <c r="F19" t="s">
-        <v>191</v>
-      </c>
-      <c r="G19" t="s">
-        <v>191</v>
-      </c>
-      <c r="H19" t="s">
-        <v>195</v>
-      </c>
-      <c r="I19" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" t="s">
         <v>197</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" t="s">
         <v>198</v>
       </c>
-      <c r="D20" t="s">
+      <c r="G20" t="s">
         <v>199</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H20" t="s">
         <v>200</v>
       </c>
-      <c r="F20" t="s">
+      <c r="I20" t="s">
         <v>201</v>
-      </c>
-      <c r="G20" t="s">
-        <v>202</v>
-      </c>
-      <c r="H20" t="s">
-        <v>203</v>
-      </c>
-      <c r="I20" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F21" t="s">
+        <v>202</v>
+      </c>
+      <c r="G21" t="s">
+        <v>202</v>
+      </c>
+      <c r="H21" t="s">
+        <v>204</v>
+      </c>
+      <c r="I21" t="s">
         <v>205</v>
-      </c>
-      <c r="C21" t="s">
-        <v>205</v>
-      </c>
-      <c r="D21" t="s">
-        <v>205</v>
-      </c>
-      <c r="E21" t="s">
-        <v>206</v>
-      </c>
-      <c r="F21" t="s">
-        <v>205</v>
-      </c>
-      <c r="G21" t="s">
-        <v>205</v>
-      </c>
-      <c r="H21" t="s">
-        <v>207</v>
-      </c>
-      <c r="I21" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="B22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" t="s">
+        <v>206</v>
+      </c>
+      <c r="E22" t="s">
+        <v>207</v>
+      </c>
+      <c r="F22" t="s">
+        <v>206</v>
+      </c>
+      <c r="G22" t="s">
+        <v>206</v>
+      </c>
+      <c r="H22" t="s">
+        <v>208</v>
+      </c>
+      <c r="I22" t="s">
         <v>209</v>
-      </c>
-      <c r="C22" t="s">
-        <v>209</v>
-      </c>
-      <c r="D22" t="s">
-        <v>209</v>
-      </c>
-      <c r="E22" t="s">
-        <v>210</v>
-      </c>
-      <c r="F22" t="s">
-        <v>209</v>
-      </c>
-      <c r="G22" t="s">
-        <v>209</v>
-      </c>
-      <c r="H22" t="s">
-        <v>211</v>
-      </c>
-      <c r="I22" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="B23" t="s">
+        <v>210</v>
+      </c>
+      <c r="C23" t="s">
+        <v>211</v>
+      </c>
+      <c r="D23" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" t="s">
         <v>213</v>
       </c>
-      <c r="C23" t="s">
+      <c r="F23" t="s">
+        <v>210</v>
+      </c>
+      <c r="G23" t="s">
+        <v>210</v>
+      </c>
+      <c r="H23" t="s">
         <v>214</v>
       </c>
-      <c r="D23" t="s">
+      <c r="I23" t="s">
         <v>215</v>
-      </c>
-      <c r="E23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F23" t="s">
-        <v>213</v>
-      </c>
-      <c r="G23" t="s">
-        <v>213</v>
-      </c>
-      <c r="H23" t="s">
-        <v>217</v>
-      </c>
-      <c r="I23" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B24" t="s">
+        <v>216</v>
+      </c>
+      <c r="C24" t="s">
+        <v>217</v>
+      </c>
+      <c r="D24" t="s">
+        <v>218</v>
+      </c>
+      <c r="E24" t="s">
         <v>219</v>
       </c>
-      <c r="C24" t="s">
+      <c r="F24" t="s">
+        <v>216</v>
+      </c>
+      <c r="G24" t="s">
+        <v>216</v>
+      </c>
+      <c r="H24" t="s">
         <v>220</v>
       </c>
-      <c r="D24" t="s">
+      <c r="I24" t="s">
         <v>221</v>
-      </c>
-      <c r="E24" t="s">
-        <v>222</v>
-      </c>
-      <c r="F24" t="s">
-        <v>219</v>
-      </c>
-      <c r="G24" t="s">
-        <v>219</v>
-      </c>
-      <c r="H24" t="s">
-        <v>223</v>
-      </c>
-      <c r="I24" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B25" t="s">
+        <v>222</v>
+      </c>
+      <c r="C25" t="s">
+        <v>223</v>
+      </c>
+      <c r="D25" t="s">
+        <v>224</v>
+      </c>
+      <c r="E25" t="s">
         <v>225</v>
       </c>
-      <c r="C25" t="s">
+      <c r="F25" t="s">
         <v>226</v>
       </c>
-      <c r="D25" t="s">
+      <c r="G25" t="s">
+        <v>226</v>
+      </c>
+      <c r="H25" t="s">
         <v>227</v>
       </c>
-      <c r="E25" t="s">
-        <v>228</v>
-      </c>
-      <c r="F25" t="s">
-        <v>229</v>
-      </c>
-      <c r="G25" t="s">
-        <v>229</v>
-      </c>
-      <c r="H25" t="s">
-        <v>230</v>
-      </c>
       <c r="I25" t="s">
-        <v>231</v>
+        <v>713</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="B26" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" t="s">
+        <v>228</v>
+      </c>
+      <c r="D26" t="s">
+        <v>228</v>
+      </c>
+      <c r="E26" t="s">
+        <v>229</v>
+      </c>
+      <c r="F26" t="s">
+        <v>230</v>
+      </c>
+      <c r="G26" t="s">
+        <v>231</v>
+      </c>
+      <c r="H26" t="s">
         <v>232</v>
       </c>
-      <c r="C26" t="s">
-        <v>232</v>
-      </c>
-      <c r="D26" t="s">
-        <v>232</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="I26" t="s">
         <v>233</v>
-      </c>
-      <c r="F26" t="s">
-        <v>234</v>
-      </c>
-      <c r="G26" t="s">
-        <v>235</v>
-      </c>
-      <c r="H26" t="s">
-        <v>236</v>
-      </c>
-      <c r="I26" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="B27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" t="s">
+        <v>235</v>
+      </c>
+      <c r="E27" t="s">
+        <v>236</v>
+      </c>
+      <c r="F27" t="s">
+        <v>237</v>
+      </c>
+      <c r="G27" t="s">
+        <v>237</v>
+      </c>
+      <c r="H27" t="s">
         <v>238</v>
       </c>
-      <c r="C27" t="s">
+      <c r="I27" t="s">
         <v>239</v>
-      </c>
-      <c r="D27" t="s">
-        <v>239</v>
-      </c>
-      <c r="E27" t="s">
-        <v>240</v>
-      </c>
-      <c r="F27" t="s">
-        <v>241</v>
-      </c>
-      <c r="G27" t="s">
-        <v>241</v>
-      </c>
-      <c r="H27" t="s">
-        <v>242</v>
-      </c>
-      <c r="I27" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B28" t="s">
+        <v>240</v>
+      </c>
+      <c r="C28" t="s">
+        <v>241</v>
+      </c>
+      <c r="D28" t="s">
+        <v>242</v>
+      </c>
+      <c r="E28" t="s">
+        <v>240</v>
+      </c>
+      <c r="F28" t="s">
+        <v>240</v>
+      </c>
+      <c r="G28" t="s">
+        <v>243</v>
+      </c>
+      <c r="H28" t="s">
         <v>244</v>
       </c>
-      <c r="C28" t="s">
+      <c r="I28" t="s">
         <v>245</v>
-      </c>
-      <c r="D28" t="s">
-        <v>246</v>
-      </c>
-      <c r="E28" t="s">
-        <v>244</v>
-      </c>
-      <c r="F28" t="s">
-        <v>244</v>
-      </c>
-      <c r="G28" t="s">
-        <v>247</v>
-      </c>
-      <c r="H28" t="s">
-        <v>248</v>
-      </c>
-      <c r="I28" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B29" t="s">
+        <v>246</v>
+      </c>
+      <c r="C29" t="s">
+        <v>246</v>
+      </c>
+      <c r="D29" t="s">
+        <v>247</v>
+      </c>
+      <c r="E29" t="s">
+        <v>248</v>
+      </c>
+      <c r="F29" t="s">
+        <v>246</v>
+      </c>
+      <c r="G29" t="s">
+        <v>248</v>
+      </c>
+      <c r="H29" t="s">
+        <v>249</v>
+      </c>
+      <c r="I29" t="s">
         <v>250</v>
-      </c>
-      <c r="C29" t="s">
-        <v>250</v>
-      </c>
-      <c r="D29" t="s">
-        <v>251</v>
-      </c>
-      <c r="E29" t="s">
-        <v>252</v>
-      </c>
-      <c r="F29" t="s">
-        <v>250</v>
-      </c>
-      <c r="G29" t="s">
-        <v>252</v>
-      </c>
-      <c r="H29" t="s">
-        <v>253</v>
-      </c>
-      <c r="I29" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="B30" t="s">
+        <v>251</v>
+      </c>
+      <c r="C30" t="s">
+        <v>252</v>
+      </c>
+      <c r="D30" t="s">
+        <v>253</v>
+      </c>
+      <c r="E30" t="s">
+        <v>254</v>
+      </c>
+      <c r="F30" t="s">
         <v>255</v>
       </c>
-      <c r="C30" t="s">
+      <c r="G30" t="s">
         <v>256</v>
       </c>
-      <c r="D30" t="s">
+      <c r="H30" t="s">
         <v>257</v>
       </c>
-      <c r="E30" t="s">
+      <c r="I30" t="s">
         <v>258</v>
-      </c>
-      <c r="F30" t="s">
-        <v>259</v>
-      </c>
-      <c r="G30" t="s">
-        <v>260</v>
-      </c>
-      <c r="H30" t="s">
-        <v>261</v>
-      </c>
-      <c r="I30" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="B31" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C31" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D31" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E31" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F31" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G31" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="H31" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="I31" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B32" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C32" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D32" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E32" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F32" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="G32" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="I32" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B33" t="s">
+        <v>265</v>
+      </c>
+      <c r="C33" t="s">
+        <v>266</v>
+      </c>
+      <c r="D33" t="s">
+        <v>267</v>
+      </c>
+      <c r="E33" t="s">
+        <v>268</v>
+      </c>
+      <c r="F33" t="s">
         <v>269</v>
       </c>
-      <c r="C33" t="s">
+      <c r="G33" t="s">
+        <v>268</v>
+      </c>
+      <c r="H33" t="s">
         <v>270</v>
       </c>
-      <c r="D33" t="s">
+      <c r="I33" t="s">
         <v>271</v>
-      </c>
-      <c r="E33" t="s">
-        <v>272</v>
-      </c>
-      <c r="F33" t="s">
-        <v>273</v>
-      </c>
-      <c r="G33" t="s">
-        <v>272</v>
-      </c>
-      <c r="H33" t="s">
-        <v>274</v>
-      </c>
-      <c r="I33" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="B34" t="s">
+        <v>272</v>
+      </c>
+      <c r="C34" t="s">
+        <v>273</v>
+      </c>
+      <c r="D34" t="s">
+        <v>274</v>
+      </c>
+      <c r="E34" t="s">
+        <v>275</v>
+      </c>
+      <c r="F34" t="s">
         <v>276</v>
       </c>
-      <c r="C34" t="s">
+      <c r="G34" t="s">
         <v>277</v>
       </c>
-      <c r="D34" t="s">
+      <c r="H34" t="s">
         <v>278</v>
       </c>
-      <c r="E34" t="s">
+      <c r="I34" t="s">
         <v>279</v>
-      </c>
-      <c r="F34" t="s">
-        <v>280</v>
-      </c>
-      <c r="G34" t="s">
-        <v>281</v>
-      </c>
-      <c r="H34" t="s">
-        <v>282</v>
-      </c>
-      <c r="I34" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="B35" t="s">
+        <v>280</v>
+      </c>
+      <c r="C35" t="s">
+        <v>280</v>
+      </c>
+      <c r="D35" t="s">
+        <v>280</v>
+      </c>
+      <c r="E35" t="s">
+        <v>281</v>
+      </c>
+      <c r="F35" t="s">
+        <v>282</v>
+      </c>
+      <c r="G35" t="s">
+        <v>283</v>
+      </c>
+      <c r="H35" t="s">
         <v>284</v>
       </c>
-      <c r="C35" t="s">
-        <v>284</v>
-      </c>
-      <c r="D35" t="s">
-        <v>284</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="I35" t="s">
         <v>285</v>
-      </c>
-      <c r="F35" t="s">
-        <v>286</v>
-      </c>
-      <c r="G35" t="s">
-        <v>287</v>
-      </c>
-      <c r="H35" t="s">
-        <v>288</v>
-      </c>
-      <c r="I35" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B36" t="s">
+        <v>286</v>
+      </c>
+      <c r="C36" t="s">
+        <v>287</v>
+      </c>
+      <c r="D36" t="s">
+        <v>286</v>
+      </c>
+      <c r="E36" t="s">
+        <v>288</v>
+      </c>
+      <c r="F36" t="s">
+        <v>289</v>
+      </c>
+      <c r="G36" t="s">
         <v>290</v>
       </c>
-      <c r="C36" t="s">
+      <c r="H36" t="s">
         <v>291</v>
       </c>
-      <c r="D36" t="s">
-        <v>290</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="I36" t="s">
         <v>292</v>
-      </c>
-      <c r="F36" t="s">
-        <v>293</v>
-      </c>
-      <c r="G36" t="s">
-        <v>294</v>
-      </c>
-      <c r="H36" t="s">
-        <v>295</v>
-      </c>
-      <c r="I36" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B37" t="s">
+        <v>293</v>
+      </c>
+      <c r="C37" t="s">
+        <v>294</v>
+      </c>
+      <c r="D37" t="s">
+        <v>293</v>
+      </c>
+      <c r="E37" t="s">
+        <v>295</v>
+      </c>
+      <c r="F37" t="s">
+        <v>296</v>
+      </c>
+      <c r="G37" t="s">
         <v>297</v>
       </c>
-      <c r="C37" t="s">
+      <c r="H37" t="s">
         <v>298</v>
       </c>
-      <c r="D37" t="s">
-        <v>297</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="I37" t="s">
         <v>299</v>
-      </c>
-      <c r="F37" t="s">
-        <v>300</v>
-      </c>
-      <c r="G37" t="s">
-        <v>301</v>
-      </c>
-      <c r="H37" t="s">
-        <v>302</v>
-      </c>
-      <c r="I37" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="B38" t="s">
+        <v>300</v>
+      </c>
+      <c r="C38" t="s">
+        <v>301</v>
+      </c>
+      <c r="D38" t="s">
+        <v>302</v>
+      </c>
+      <c r="E38" t="s">
+        <v>303</v>
+      </c>
+      <c r="F38" t="s">
         <v>304</v>
       </c>
-      <c r="C38" t="s">
+      <c r="G38" t="s">
         <v>305</v>
       </c>
-      <c r="D38" t="s">
+      <c r="H38" t="s">
         <v>306</v>
       </c>
-      <c r="E38" t="s">
+      <c r="I38" t="s">
         <v>307</v>
-      </c>
-      <c r="F38" t="s">
-        <v>308</v>
-      </c>
-      <c r="G38" t="s">
-        <v>309</v>
-      </c>
-      <c r="H38" t="s">
-        <v>310</v>
-      </c>
-      <c r="I38" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B39" t="s">
+        <v>308</v>
+      </c>
+      <c r="C39" t="s">
+        <v>309</v>
+      </c>
+      <c r="D39" t="s">
+        <v>308</v>
+      </c>
+      <c r="E39" t="s">
+        <v>308</v>
+      </c>
+      <c r="F39" t="s">
+        <v>310</v>
+      </c>
+      <c r="G39" t="s">
+        <v>308</v>
+      </c>
+      <c r="H39" t="s">
+        <v>311</v>
+      </c>
+      <c r="I39" t="s">
         <v>312</v>
-      </c>
-      <c r="C39" t="s">
-        <v>313</v>
-      </c>
-      <c r="D39" t="s">
-        <v>312</v>
-      </c>
-      <c r="E39" t="s">
-        <v>312</v>
-      </c>
-      <c r="F39" t="s">
-        <v>314</v>
-      </c>
-      <c r="G39" t="s">
-        <v>312</v>
-      </c>
-      <c r="H39" t="s">
-        <v>315</v>
-      </c>
-      <c r="I39" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B40" t="s">
+        <v>313</v>
+      </c>
+      <c r="C40" t="s">
+        <v>314</v>
+      </c>
+      <c r="D40" t="s">
+        <v>315</v>
+      </c>
+      <c r="E40" t="s">
+        <v>316</v>
+      </c>
+      <c r="F40" t="s">
         <v>317</v>
       </c>
-      <c r="C40" t="s">
+      <c r="G40" t="s">
         <v>318</v>
       </c>
-      <c r="D40" t="s">
+      <c r="H40" t="s">
         <v>319</v>
       </c>
-      <c r="E40" t="s">
+      <c r="I40" t="s">
         <v>320</v>
-      </c>
-      <c r="F40" t="s">
-        <v>321</v>
-      </c>
-      <c r="G40" t="s">
-        <v>322</v>
-      </c>
-      <c r="H40" t="s">
-        <v>323</v>
-      </c>
-      <c r="I40" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B41" t="s">
+        <v>321</v>
+      </c>
+      <c r="C41" t="s">
+        <v>322</v>
+      </c>
+      <c r="D41" t="s">
+        <v>323</v>
+      </c>
+      <c r="E41" t="s">
+        <v>324</v>
+      </c>
+      <c r="F41" t="s">
         <v>325</v>
       </c>
-      <c r="C41" t="s">
+      <c r="G41" t="s">
         <v>326</v>
       </c>
-      <c r="D41" t="s">
+      <c r="H41" t="s">
         <v>327</v>
       </c>
-      <c r="E41" t="s">
+      <c r="I41" t="s">
         <v>328</v>
-      </c>
-      <c r="F41" t="s">
-        <v>329</v>
-      </c>
-      <c r="G41" t="s">
-        <v>330</v>
-      </c>
-      <c r="H41" t="s">
-        <v>331</v>
-      </c>
-      <c r="I41" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="B42" t="s">
+        <v>329</v>
+      </c>
+      <c r="C42" t="s">
+        <v>330</v>
+      </c>
+      <c r="D42" t="s">
+        <v>331</v>
+      </c>
+      <c r="E42" t="s">
+        <v>332</v>
+      </c>
+      <c r="F42" t="s">
         <v>333</v>
       </c>
-      <c r="C42" t="s">
+      <c r="G42" t="s">
         <v>334</v>
       </c>
-      <c r="D42" t="s">
+      <c r="H42" t="s">
         <v>335</v>
       </c>
-      <c r="E42" t="s">
+      <c r="I42" t="s">
         <v>336</v>
-      </c>
-      <c r="F42" t="s">
-        <v>337</v>
-      </c>
-      <c r="G42" t="s">
-        <v>338</v>
-      </c>
-      <c r="H42" t="s">
-        <v>339</v>
-      </c>
-      <c r="I42" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B43" t="s">
+        <v>337</v>
+      </c>
+      <c r="C43" t="s">
+        <v>337</v>
+      </c>
+      <c r="D43" t="s">
+        <v>337</v>
+      </c>
+      <c r="E43" t="s">
+        <v>338</v>
+      </c>
+      <c r="F43" t="s">
+        <v>339</v>
+      </c>
+      <c r="G43" t="s">
+        <v>340</v>
+      </c>
+      <c r="H43" t="s">
         <v>341</v>
       </c>
-      <c r="C43" t="s">
-        <v>341</v>
-      </c>
-      <c r="D43" t="s">
-        <v>341</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="I43" t="s">
         <v>342</v>
-      </c>
-      <c r="F43" t="s">
-        <v>343</v>
-      </c>
-      <c r="G43" t="s">
-        <v>344</v>
-      </c>
-      <c r="H43" t="s">
-        <v>345</v>
-      </c>
-      <c r="I43" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="B44" t="s">
+        <v>343</v>
+      </c>
+      <c r="C44" t="s">
+        <v>344</v>
+      </c>
+      <c r="D44" t="s">
+        <v>345</v>
+      </c>
+      <c r="E44" t="s">
+        <v>346</v>
+      </c>
+      <c r="F44" t="s">
         <v>347</v>
       </c>
-      <c r="C44" t="s">
+      <c r="G44" t="s">
         <v>348</v>
       </c>
-      <c r="D44" t="s">
+      <c r="H44" t="s">
         <v>349</v>
       </c>
-      <c r="E44" t="s">
+      <c r="I44" t="s">
         <v>350</v>
-      </c>
-      <c r="F44" t="s">
-        <v>351</v>
-      </c>
-      <c r="G44" t="s">
-        <v>352</v>
-      </c>
-      <c r="H44" t="s">
-        <v>353</v>
-      </c>
-      <c r="I44" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="B45" t="s">
+        <v>351</v>
+      </c>
+      <c r="C45" t="s">
+        <v>352</v>
+      </c>
+      <c r="D45" t="s">
+        <v>351</v>
+      </c>
+      <c r="E45" t="s">
+        <v>353</v>
+      </c>
+      <c r="F45" t="s">
+        <v>354</v>
+      </c>
+      <c r="G45" t="s">
         <v>355</v>
       </c>
-      <c r="C45" t="s">
+      <c r="H45" t="s">
         <v>356</v>
       </c>
-      <c r="D45" t="s">
-        <v>355</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="I45" t="s">
         <v>357</v>
-      </c>
-      <c r="F45" t="s">
-        <v>358</v>
-      </c>
-      <c r="G45" t="s">
-        <v>359</v>
-      </c>
-      <c r="H45" t="s">
-        <v>360</v>
-      </c>
-      <c r="I45" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="B46" t="s">
+        <v>358</v>
+      </c>
+      <c r="C46" t="s">
+        <v>359</v>
+      </c>
+      <c r="D46" t="s">
+        <v>360</v>
+      </c>
+      <c r="E46" t="s">
+        <v>361</v>
+      </c>
+      <c r="F46" t="s">
         <v>362</v>
       </c>
-      <c r="C46" t="s">
+      <c r="G46" t="s">
         <v>363</v>
       </c>
-      <c r="D46" t="s">
+      <c r="H46" t="s">
         <v>364</v>
       </c>
-      <c r="E46" t="s">
+      <c r="I46" t="s">
         <v>365</v>
-      </c>
-      <c r="F46" t="s">
-        <v>366</v>
-      </c>
-      <c r="G46" t="s">
-        <v>367</v>
-      </c>
-      <c r="H46" t="s">
-        <v>368</v>
-      </c>
-      <c r="I46" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B47" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C47" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D47" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E47" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F47" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="G47" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="H47" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="I47" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="B48" t="s">
+        <v>370</v>
+      </c>
+      <c r="C48" t="s">
+        <v>371</v>
+      </c>
+      <c r="D48" t="s">
+        <v>371</v>
+      </c>
+      <c r="E48" t="s">
+        <v>372</v>
+      </c>
+      <c r="F48" t="s">
+        <v>373</v>
+      </c>
+      <c r="G48" t="s">
         <v>374</v>
       </c>
-      <c r="C48" t="s">
+      <c r="H48" t="s">
         <v>375</v>
       </c>
-      <c r="D48" t="s">
-        <v>375</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="I48" t="s">
         <v>376</v>
-      </c>
-      <c r="F48" t="s">
-        <v>377</v>
-      </c>
-      <c r="G48" t="s">
-        <v>378</v>
-      </c>
-      <c r="H48" t="s">
-        <v>379</v>
-      </c>
-      <c r="I48" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="B49" t="s">
+        <v>377</v>
+      </c>
+      <c r="C49" t="s">
+        <v>378</v>
+      </c>
+      <c r="D49" t="s">
+        <v>377</v>
+      </c>
+      <c r="E49" t="s">
+        <v>379</v>
+      </c>
+      <c r="F49" t="s">
+        <v>380</v>
+      </c>
+      <c r="G49" t="s">
         <v>381</v>
       </c>
-      <c r="C49" t="s">
+      <c r="H49" t="s">
         <v>382</v>
       </c>
-      <c r="D49" t="s">
-        <v>381</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="I49" t="s">
         <v>383</v>
-      </c>
-      <c r="F49" t="s">
-        <v>384</v>
-      </c>
-      <c r="G49" t="s">
-        <v>385</v>
-      </c>
-      <c r="H49" t="s">
-        <v>386</v>
-      </c>
-      <c r="I49" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="B50" t="s">
+        <v>384</v>
+      </c>
+      <c r="C50" t="s">
+        <v>385</v>
+      </c>
+      <c r="D50" t="s">
+        <v>385</v>
+      </c>
+      <c r="E50" t="s">
+        <v>386</v>
+      </c>
+      <c r="F50" t="s">
+        <v>387</v>
+      </c>
+      <c r="G50" t="s">
         <v>388</v>
       </c>
-      <c r="C50" t="s">
+      <c r="H50" t="s">
         <v>389</v>
       </c>
-      <c r="D50" t="s">
-        <v>389</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="I50" t="s">
         <v>390</v>
-      </c>
-      <c r="F50" t="s">
-        <v>391</v>
-      </c>
-      <c r="G50" t="s">
-        <v>392</v>
-      </c>
-      <c r="H50" t="s">
-        <v>393</v>
-      </c>
-      <c r="I50" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="B51" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C51" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D51" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E51" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="F51" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G51" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H51" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I51" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B52" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C52" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D52" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E52" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="F52" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="G52" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="H52" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="I52" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B53" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C53" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D53" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E53" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="F53" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="G53" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="H53" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="I53" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="B54" t="s">
+        <v>401</v>
+      </c>
+      <c r="C54" t="s">
+        <v>402</v>
+      </c>
+      <c r="D54" t="s">
+        <v>403</v>
+      </c>
+      <c r="E54" t="s">
+        <v>404</v>
+      </c>
+      <c r="F54" t="s">
         <v>405</v>
       </c>
-      <c r="C54" t="s">
+      <c r="G54" t="s">
         <v>406</v>
       </c>
-      <c r="D54" t="s">
+      <c r="H54" t="s">
         <v>407</v>
       </c>
-      <c r="E54" t="s">
+      <c r="I54" t="s">
         <v>408</v>
-      </c>
-      <c r="F54" t="s">
-        <v>409</v>
-      </c>
-      <c r="G54" t="s">
-        <v>410</v>
-      </c>
-      <c r="H54" t="s">
-        <v>411</v>
-      </c>
-      <c r="I54" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B55" t="s">
+        <v>409</v>
+      </c>
+      <c r="C55" t="s">
+        <v>410</v>
+      </c>
+      <c r="D55" t="s">
+        <v>411</v>
+      </c>
+      <c r="E55" t="s">
+        <v>412</v>
+      </c>
+      <c r="F55" t="s">
         <v>413</v>
       </c>
-      <c r="C55" t="s">
+      <c r="G55" t="s">
         <v>414</v>
       </c>
-      <c r="D55" t="s">
+      <c r="H55" t="s">
         <v>415</v>
       </c>
-      <c r="E55" t="s">
+      <c r="I55" t="s">
         <v>416</v>
-      </c>
-      <c r="F55" t="s">
-        <v>417</v>
-      </c>
-      <c r="G55" t="s">
-        <v>418</v>
-      </c>
-      <c r="H55" t="s">
-        <v>419</v>
-      </c>
-      <c r="I55" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B56" t="s">
+        <v>417</v>
+      </c>
+      <c r="C56" t="s">
+        <v>418</v>
+      </c>
+      <c r="D56" t="s">
+        <v>418</v>
+      </c>
+      <c r="E56" t="s">
+        <v>419</v>
+      </c>
+      <c r="F56" t="s">
+        <v>420</v>
+      </c>
+      <c r="G56" t="s">
         <v>421</v>
       </c>
-      <c r="C56" t="s">
+      <c r="H56" t="s">
         <v>422</v>
       </c>
-      <c r="D56" t="s">
-        <v>422</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="I56" t="s">
         <v>423</v>
-      </c>
-      <c r="F56" t="s">
-        <v>424</v>
-      </c>
-      <c r="G56" t="s">
-        <v>425</v>
-      </c>
-      <c r="H56" t="s">
-        <v>426</v>
-      </c>
-      <c r="I56" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B57" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C57" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D57" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="E57" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="F57" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G57" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H57" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="I57" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="B58" t="s">
+        <v>427</v>
+      </c>
+      <c r="C58" t="s">
+        <v>428</v>
+      </c>
+      <c r="D58" t="s">
+        <v>428</v>
+      </c>
+      <c r="E58" t="s">
+        <v>429</v>
+      </c>
+      <c r="F58" t="s">
+        <v>430</v>
+      </c>
+      <c r="G58" t="s">
+        <v>427</v>
+      </c>
+      <c r="H58" t="s">
         <v>431</v>
       </c>
-      <c r="C58" t="s">
+      <c r="I58" t="s">
         <v>432</v>
-      </c>
-      <c r="D58" t="s">
-        <v>432</v>
-      </c>
-      <c r="E58" t="s">
-        <v>433</v>
-      </c>
-      <c r="F58" t="s">
-        <v>434</v>
-      </c>
-      <c r="G58" t="s">
-        <v>431</v>
-      </c>
-      <c r="H58" t="s">
-        <v>435</v>
-      </c>
-      <c r="I58" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B59" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C59" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D59" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="E59" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F59" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="G59" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="H59" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="I59" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B60" t="s">
+        <v>436</v>
+      </c>
+      <c r="C60" t="s">
+        <v>437</v>
+      </c>
+      <c r="D60" t="s">
+        <v>438</v>
+      </c>
+      <c r="E60" t="s">
+        <v>439</v>
+      </c>
+      <c r="F60" t="s">
         <v>440</v>
       </c>
-      <c r="C60" t="s">
+      <c r="G60" t="s">
         <v>441</v>
       </c>
-      <c r="D60" t="s">
+      <c r="H60" t="s">
         <v>442</v>
       </c>
-      <c r="E60" t="s">
+      <c r="I60" t="s">
         <v>443</v>
-      </c>
-      <c r="F60" t="s">
-        <v>444</v>
-      </c>
-      <c r="G60" t="s">
-        <v>445</v>
-      </c>
-      <c r="H60" t="s">
-        <v>446</v>
-      </c>
-      <c r="I60" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A61" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="B61" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C61" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D61" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="E61" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="F61" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G61" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="H61" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="I61" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B62" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C62" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D62" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E62" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="F62" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G62" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="H62" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="I62" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B63" t="s">
+        <v>451</v>
+      </c>
+      <c r="C63" t="s">
+        <v>452</v>
+      </c>
+      <c r="D63" t="s">
+        <v>453</v>
+      </c>
+      <c r="E63" t="s">
+        <v>454</v>
+      </c>
+      <c r="F63" t="s">
         <v>455</v>
       </c>
-      <c r="C63" t="s">
+      <c r="G63" t="s">
         <v>456</v>
       </c>
-      <c r="D63" t="s">
+      <c r="H63" t="s">
         <v>457</v>
       </c>
-      <c r="E63" t="s">
+      <c r="I63" t="s">
         <v>458</v>
-      </c>
-      <c r="F63" t="s">
-        <v>459</v>
-      </c>
-      <c r="G63" t="s">
-        <v>460</v>
-      </c>
-      <c r="H63" t="s">
-        <v>461</v>
-      </c>
-      <c r="I63" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="B64" t="s">
+        <v>459</v>
+      </c>
+      <c r="C64" t="s">
+        <v>460</v>
+      </c>
+      <c r="D64" t="s">
+        <v>461</v>
+      </c>
+      <c r="E64" t="s">
+        <v>462</v>
+      </c>
+      <c r="F64" t="s">
         <v>463</v>
       </c>
-      <c r="C64" t="s">
+      <c r="G64" t="s">
         <v>464</v>
       </c>
-      <c r="D64" t="s">
+      <c r="H64" t="s">
         <v>465</v>
       </c>
-      <c r="E64" t="s">
+      <c r="I64" t="s">
         <v>466</v>
-      </c>
-      <c r="F64" t="s">
-        <v>467</v>
-      </c>
-      <c r="G64" t="s">
-        <v>468</v>
-      </c>
-      <c r="H64" t="s">
-        <v>469</v>
-      </c>
-      <c r="I64" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="B65" t="s">
+        <v>467</v>
+      </c>
+      <c r="C65" t="s">
+        <v>467</v>
+      </c>
+      <c r="D65" t="s">
+        <v>468</v>
+      </c>
+      <c r="E65" t="s">
+        <v>469</v>
+      </c>
+      <c r="F65" t="s">
+        <v>470</v>
+      </c>
+      <c r="G65" t="s">
+        <v>467</v>
+      </c>
+      <c r="H65" t="s">
         <v>471</v>
       </c>
-      <c r="C65" t="s">
-        <v>471</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="I65" t="s">
         <v>472</v>
-      </c>
-      <c r="E65" t="s">
-        <v>473</v>
-      </c>
-      <c r="F65" t="s">
-        <v>474</v>
-      </c>
-      <c r="G65" t="s">
-        <v>471</v>
-      </c>
-      <c r="H65" t="s">
-        <v>475</v>
-      </c>
-      <c r="I65" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="B66" t="s">
+        <v>473</v>
+      </c>
+      <c r="C66" t="s">
+        <v>474</v>
+      </c>
+      <c r="D66" t="s">
+        <v>473</v>
+      </c>
+      <c r="E66" t="s">
+        <v>475</v>
+      </c>
+      <c r="F66" t="s">
+        <v>476</v>
+      </c>
+      <c r="G66" t="s">
         <v>477</v>
       </c>
-      <c r="C66" t="s">
+      <c r="H66" t="s">
         <v>478</v>
       </c>
-      <c r="D66" t="s">
-        <v>477</v>
-      </c>
-      <c r="E66" t="s">
+      <c r="I66" t="s">
         <v>479</v>
-      </c>
-      <c r="F66" t="s">
-        <v>480</v>
-      </c>
-      <c r="G66" t="s">
-        <v>481</v>
-      </c>
-      <c r="H66" t="s">
-        <v>482</v>
-      </c>
-      <c r="I66" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B67" t="s">
+        <v>480</v>
+      </c>
+      <c r="C67" t="s">
+        <v>480</v>
+      </c>
+      <c r="D67" t="s">
+        <v>480</v>
+      </c>
+      <c r="E67" t="s">
+        <v>481</v>
+      </c>
+      <c r="F67" t="s">
+        <v>482</v>
+      </c>
+      <c r="G67" t="s">
+        <v>483</v>
+      </c>
+      <c r="H67" t="s">
         <v>484</v>
       </c>
-      <c r="C67" t="s">
-        <v>484</v>
-      </c>
-      <c r="D67" t="s">
-        <v>484</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="I67" t="s">
         <v>485</v>
-      </c>
-      <c r="F67" t="s">
-        <v>486</v>
-      </c>
-      <c r="G67" t="s">
-        <v>487</v>
-      </c>
-      <c r="H67" t="s">
-        <v>488</v>
-      </c>
-      <c r="I67" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B68" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C68" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="D68" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E68" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F68" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G68" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="H68" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="I68" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="B69" t="s">
+        <v>490</v>
+      </c>
+      <c r="C69" t="s">
+        <v>491</v>
+      </c>
+      <c r="D69" t="s">
+        <v>492</v>
+      </c>
+      <c r="E69" t="s">
+        <v>493</v>
+      </c>
+      <c r="F69" t="s">
         <v>494</v>
       </c>
-      <c r="C69" t="s">
+      <c r="G69" t="s">
         <v>495</v>
       </c>
-      <c r="D69" t="s">
+      <c r="H69" t="s">
         <v>496</v>
       </c>
-      <c r="E69" t="s">
+      <c r="I69" t="s">
         <v>497</v>
-      </c>
-      <c r="F69" t="s">
-        <v>498</v>
-      </c>
-      <c r="G69" t="s">
-        <v>499</v>
-      </c>
-      <c r="H69" t="s">
-        <v>500</v>
-      </c>
-      <c r="I69" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="B70" t="s">
+        <v>498</v>
+      </c>
+      <c r="C70" t="s">
+        <v>499</v>
+      </c>
+      <c r="D70" t="s">
+        <v>500</v>
+      </c>
+      <c r="E70" t="s">
+        <v>501</v>
+      </c>
+      <c r="F70" t="s">
         <v>502</v>
       </c>
-      <c r="C70" t="s">
+      <c r="G70" t="s">
         <v>503</v>
       </c>
-      <c r="D70" t="s">
+      <c r="H70" t="s">
         <v>504</v>
       </c>
-      <c r="E70" t="s">
+      <c r="I70" t="s">
         <v>505</v>
-      </c>
-      <c r="F70" t="s">
-        <v>506</v>
-      </c>
-      <c r="G70" t="s">
-        <v>507</v>
-      </c>
-      <c r="H70" t="s">
-        <v>508</v>
-      </c>
-      <c r="I70" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B71" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C71" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D71" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="E71" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="F71" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="G71" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="H71" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="I71" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A72" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="B72" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C72" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D72" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="E72" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="F72" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G72" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="H72" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="I72" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="B73" t="s">
+        <v>514</v>
+      </c>
+      <c r="C73" t="s">
+        <v>514</v>
+      </c>
+      <c r="D73" t="s">
+        <v>514</v>
+      </c>
+      <c r="E73" t="s">
+        <v>515</v>
+      </c>
+      <c r="F73" t="s">
+        <v>516</v>
+      </c>
+      <c r="G73" t="s">
+        <v>517</v>
+      </c>
+      <c r="H73" t="s">
         <v>518</v>
       </c>
-      <c r="C73" t="s">
-        <v>518</v>
-      </c>
-      <c r="D73" t="s">
-        <v>518</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="I73" t="s">
         <v>519</v>
-      </c>
-      <c r="F73" t="s">
-        <v>520</v>
-      </c>
-      <c r="G73" t="s">
-        <v>521</v>
-      </c>
-      <c r="H73" t="s">
-        <v>522</v>
-      </c>
-      <c r="I73" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B74" t="s">
+        <v>520</v>
+      </c>
+      <c r="C74" t="s">
+        <v>520</v>
+      </c>
+      <c r="D74" t="s">
+        <v>521</v>
+      </c>
+      <c r="E74" t="s">
+        <v>522</v>
+      </c>
+      <c r="F74" t="s">
+        <v>520</v>
+      </c>
+      <c r="G74" t="s">
+        <v>522</v>
+      </c>
+      <c r="H74" t="s">
+        <v>523</v>
+      </c>
+      <c r="I74" t="s">
         <v>524</v>
-      </c>
-      <c r="C74" t="s">
-        <v>524</v>
-      </c>
-      <c r="D74" t="s">
-        <v>525</v>
-      </c>
-      <c r="E74" t="s">
-        <v>526</v>
-      </c>
-      <c r="F74" t="s">
-        <v>524</v>
-      </c>
-      <c r="G74" t="s">
-        <v>526</v>
-      </c>
-      <c r="H74" t="s">
-        <v>527</v>
-      </c>
-      <c r="I74" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B75" t="s">
+        <v>525</v>
+      </c>
+      <c r="C75" t="s">
+        <v>525</v>
+      </c>
+      <c r="D75" t="s">
+        <v>526</v>
+      </c>
+      <c r="E75" t="s">
+        <v>527</v>
+      </c>
+      <c r="F75" t="s">
+        <v>525</v>
+      </c>
+      <c r="G75" t="s">
+        <v>525</v>
+      </c>
+      <c r="H75" t="s">
+        <v>528</v>
+      </c>
+      <c r="I75" t="s">
         <v>529</v>
-      </c>
-      <c r="C75" t="s">
-        <v>529</v>
-      </c>
-      <c r="D75" t="s">
-        <v>530</v>
-      </c>
-      <c r="E75" t="s">
-        <v>531</v>
-      </c>
-      <c r="F75" t="s">
-        <v>529</v>
-      </c>
-      <c r="G75" t="s">
-        <v>529</v>
-      </c>
-      <c r="H75" t="s">
-        <v>532</v>
-      </c>
-      <c r="I75" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B76" t="s">
+        <v>530</v>
+      </c>
+      <c r="C76" t="s">
+        <v>530</v>
+      </c>
+      <c r="D76" t="s">
+        <v>530</v>
+      </c>
+      <c r="E76" t="s">
+        <v>531</v>
+      </c>
+      <c r="F76" t="s">
+        <v>532</v>
+      </c>
+      <c r="G76" t="s">
+        <v>533</v>
+      </c>
+      <c r="H76" t="s">
         <v>534</v>
       </c>
-      <c r="C76" t="s">
-        <v>534</v>
-      </c>
-      <c r="D76" t="s">
-        <v>534</v>
-      </c>
-      <c r="E76" t="s">
+      <c r="I76" t="s">
         <v>535</v>
-      </c>
-      <c r="F76" t="s">
-        <v>536</v>
-      </c>
-      <c r="G76" t="s">
-        <v>537</v>
-      </c>
-      <c r="H76" t="s">
-        <v>538</v>
-      </c>
-      <c r="I76" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="B77" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C77" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="D77" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E77" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="F77" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="G77" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="H77" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="I77" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B78" t="s">
+        <v>539</v>
+      </c>
+      <c r="C78" t="s">
+        <v>540</v>
+      </c>
+      <c r="D78" t="s">
+        <v>539</v>
+      </c>
+      <c r="E78" t="s">
+        <v>541</v>
+      </c>
+      <c r="F78" t="s">
+        <v>539</v>
+      </c>
+      <c r="G78" t="s">
+        <v>540</v>
+      </c>
+      <c r="H78" t="s">
+        <v>542</v>
+      </c>
+      <c r="I78" t="s">
         <v>543</v>
-      </c>
-      <c r="C78" t="s">
-        <v>544</v>
-      </c>
-      <c r="D78" t="s">
-        <v>543</v>
-      </c>
-      <c r="E78" t="s">
-        <v>545</v>
-      </c>
-      <c r="F78" t="s">
-        <v>543</v>
-      </c>
-      <c r="G78" t="s">
-        <v>544</v>
-      </c>
-      <c r="H78" t="s">
-        <v>546</v>
-      </c>
-      <c r="I78" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A79" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="B79" t="s">
+        <v>544</v>
+      </c>
+      <c r="C79" t="s">
+        <v>544</v>
+      </c>
+      <c r="D79" t="s">
+        <v>544</v>
+      </c>
+      <c r="E79" t="s">
+        <v>545</v>
+      </c>
+      <c r="F79" t="s">
+        <v>546</v>
+      </c>
+      <c r="G79" t="s">
+        <v>547</v>
+      </c>
+      <c r="H79" t="s">
         <v>548</v>
       </c>
-      <c r="C79" t="s">
-        <v>548</v>
-      </c>
-      <c r="D79" t="s">
-        <v>548</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="I79" t="s">
         <v>549</v>
-      </c>
-      <c r="F79" t="s">
-        <v>550</v>
-      </c>
-      <c r="G79" t="s">
-        <v>551</v>
-      </c>
-      <c r="H79" t="s">
-        <v>552</v>
-      </c>
-      <c r="I79" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A80" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B80" t="s">
+        <v>550</v>
+      </c>
+      <c r="C80" t="s">
+        <v>551</v>
+      </c>
+      <c r="D80" t="s">
+        <v>552</v>
+      </c>
+      <c r="E80" t="s">
+        <v>553</v>
+      </c>
+      <c r="F80" t="s">
         <v>554</v>
       </c>
-      <c r="C80" t="s">
+      <c r="G80" t="s">
         <v>555</v>
       </c>
-      <c r="D80" t="s">
+      <c r="H80" t="s">
         <v>556</v>
       </c>
-      <c r="E80" t="s">
+      <c r="I80" t="s">
         <v>557</v>
-      </c>
-      <c r="F80" t="s">
-        <v>558</v>
-      </c>
-      <c r="G80" t="s">
-        <v>559</v>
-      </c>
-      <c r="H80" t="s">
-        <v>560</v>
-      </c>
-      <c r="I80" t="s">
-        <v>561</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
womens world cup 2023 data
</commit_message>
<xml_diff>
--- a/fonts/localization.xlsx
+++ b/fonts/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\fonts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F88856-5FA2-426E-8F01-066C4F147018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1CD5E1-E51E-4E55-AA4B-EEB499E944CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="1613" yWindow="1900" windowWidth="19200" windowHeight="10020" activeTab="6" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonts" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="748">
   <si>
     <t>key</t>
   </si>
@@ -2198,6 +2198,105 @@
   </si>
   <si>
     <t>match.score</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Nueva Zelanda</t>
+  </si>
+  <si>
+    <t>Nuova Zelanda</t>
+  </si>
+  <si>
+    <t>Nouvelle-Zélande</t>
+  </si>
+  <si>
+    <t>Neuseeland</t>
+  </si>
+  <si>
+    <t>Nieuw-Zeeland</t>
+  </si>
+  <si>
+    <t>ニュージーランド</t>
+  </si>
+  <si>
+    <t>نیوزلند</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Filipinas</t>
+  </si>
+  <si>
+    <t>Filippine</t>
+  </si>
+  <si>
+    <t>Philippinen</t>
+  </si>
+  <si>
+    <t>Filippijnen</t>
+  </si>
+  <si>
+    <t>フィリピン</t>
+  </si>
+  <si>
+    <t>وابسته به فیلیپین</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zambie</t>
+  </si>
+  <si>
+    <t>Sambia</t>
+  </si>
+  <si>
+    <t>ザンビア</t>
+  </si>
+  <si>
+    <t>زامبیا</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Haití</t>
+  </si>
+  <si>
+    <t>Haïti</t>
+  </si>
+  <si>
+    <t>ハイチ</t>
+  </si>
+  <si>
+    <t>هائیتی</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>ベトナム</t>
+  </si>
+  <si>
+    <t>ویتنام</t>
+  </si>
+  <si>
+    <t>nzl</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>zam</t>
+  </si>
+  <si>
+    <t>hai</t>
+  </si>
+  <si>
+    <t>vie</t>
   </si>
 </sst>
 </file>
@@ -2395,8 +2494,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}" name="Table6" displayName="Table6" ref="A1:I80" totalsRowShown="0">
-  <autoFilter ref="A1:I80" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}" name="Table6" displayName="Table6" ref="A1:I85" totalsRowShown="0">
+  <autoFilter ref="A1:I85" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2E55F9A9-3EF2-4534-84B5-0331227CCA52}" name="key"/>
     <tableColumn id="2" xr3:uid="{AAAAE7A0-7BF8-498D-8AB7-8D288BC7367E}" name="en"/>
@@ -2711,7 +2810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4B28FF-857C-4B73-BD2F-84CA03D2F2FC}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -3757,13 +3856,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5C7B9E-E03D-420F-8955-42B4860CC822}">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomRight" activeCell="A81" sqref="A81:A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -6098,6 +6197,151 @@
         <v>557</v>
       </c>
     </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A81" t="s">
+        <v>743</v>
+      </c>
+      <c r="B81" t="s">
+        <v>715</v>
+      </c>
+      <c r="C81" t="s">
+        <v>716</v>
+      </c>
+      <c r="D81" t="s">
+        <v>717</v>
+      </c>
+      <c r="E81" t="s">
+        <v>718</v>
+      </c>
+      <c r="F81" t="s">
+        <v>719</v>
+      </c>
+      <c r="G81" t="s">
+        <v>720</v>
+      </c>
+      <c r="H81" t="s">
+        <v>721</v>
+      </c>
+      <c r="I81" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A82" t="s">
+        <v>744</v>
+      </c>
+      <c r="B82" t="s">
+        <v>723</v>
+      </c>
+      <c r="C82" t="s">
+        <v>724</v>
+      </c>
+      <c r="D82" t="s">
+        <v>725</v>
+      </c>
+      <c r="E82" t="s">
+        <v>723</v>
+      </c>
+      <c r="F82" t="s">
+        <v>726</v>
+      </c>
+      <c r="G82" t="s">
+        <v>727</v>
+      </c>
+      <c r="H82" t="s">
+        <v>728</v>
+      </c>
+      <c r="I82" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A83" t="s">
+        <v>745</v>
+      </c>
+      <c r="B83" t="s">
+        <v>730</v>
+      </c>
+      <c r="C83" t="s">
+        <v>730</v>
+      </c>
+      <c r="D83" t="s">
+        <v>730</v>
+      </c>
+      <c r="E83" t="s">
+        <v>731</v>
+      </c>
+      <c r="F83" t="s">
+        <v>732</v>
+      </c>
+      <c r="G83" t="s">
+        <v>730</v>
+      </c>
+      <c r="H83" t="s">
+        <v>733</v>
+      </c>
+      <c r="I83" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A84" t="s">
+        <v>746</v>
+      </c>
+      <c r="B84" t="s">
+        <v>735</v>
+      </c>
+      <c r="C84" t="s">
+        <v>736</v>
+      </c>
+      <c r="D84" t="s">
+        <v>735</v>
+      </c>
+      <c r="E84" t="s">
+        <v>737</v>
+      </c>
+      <c r="F84" t="s">
+        <v>735</v>
+      </c>
+      <c r="G84" t="s">
+        <v>737</v>
+      </c>
+      <c r="H84" t="s">
+        <v>738</v>
+      </c>
+      <c r="I84" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A85" t="s">
+        <v>747</v>
+      </c>
+      <c r="B85" t="s">
+        <v>740</v>
+      </c>
+      <c r="C85" t="s">
+        <v>740</v>
+      </c>
+      <c r="D85" t="s">
+        <v>740</v>
+      </c>
+      <c r="E85" t="s">
+        <v>740</v>
+      </c>
+      <c r="F85" t="s">
+        <v>740</v>
+      </c>
+      <c r="G85" t="s">
+        <v>740</v>
+      </c>
+      <c r="H85" t="s">
+        <v>741</v>
+      </c>
+      <c r="I85" t="s">
+        <v>742</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
2023 womens cup - colors to tourney db - better releases - 2023 release
</commit_message>
<xml_diff>
--- a/fonts/localization.xlsx
+++ b/fonts/localization.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\fonts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1CD5E1-E51E-4E55-AA4B-EEB499E944CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2123BB-7EA5-4A80-B59D-51A9C54C2375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1613" yWindow="1900" windowWidth="19200" windowHeight="10020" activeTab="6" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="2567" yWindow="2567" windowWidth="19200" windowHeight="10073" activeTab="1" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonts" sheetId="6" r:id="rId1"/>
-    <sheet name="Colors" sheetId="7" r:id="rId2"/>
-    <sheet name="Page" sheetId="1" r:id="rId3"/>
-    <sheet name="Stage" sheetId="4" r:id="rId4"/>
-    <sheet name="Group" sheetId="3" r:id="rId5"/>
-    <sheet name="Match" sheetId="2" r:id="rId6"/>
-    <sheet name="Team" sheetId="5" r:id="rId7"/>
+    <sheet name="Page" sheetId="1" r:id="rId2"/>
+    <sheet name="Stage" sheetId="4" r:id="rId3"/>
+    <sheet name="Group" sheetId="3" r:id="rId4"/>
+    <sheet name="Match" sheetId="2" r:id="rId5"/>
+    <sheet name="Team" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="733">
   <si>
     <t>key</t>
   </si>
@@ -2134,54 +2133,6 @@
     <t>失点</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>#94d9f5</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>#fee289</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>#f79d8f</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>#c4e1b5</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>#b0d0ee</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>#c0e4df</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>#fab077</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>#eecbef</t>
-  </si>
-  <si>
     <t>calendar.day-of-week</t>
   </si>
   <si>
@@ -2297,6 +2248,9 @@
   </si>
   <si>
     <t>vie</t>
+  </si>
+  <si>
+    <t>{label}: ‪{timezone}</t>
   </si>
 </sst>
 </file>
@@ -2403,24 +2357,6 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{929CEE80-3E9F-45B9-B9D8-C06C38A7D0B3}" name="groups" displayName="groups" ref="A1:I9" totalsRowShown="0">
-  <autoFilter ref="A1:I9" xr:uid="{4B86982E-77B7-4963-838F-4D594C24841B}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D0E0E528-2BCB-4298-80EB-394686B036E7}" name="key"/>
-    <tableColumn id="2" xr3:uid="{3AD006A1-BF1D-4EE6-A45C-16FF2881DC52}" name="en"/>
-    <tableColumn id="3" xr3:uid="{26579E3F-BC15-4480-AD0D-BD2B2AE4B0AF}" name="es"/>
-    <tableColumn id="4" xr3:uid="{8BAB4BAD-FFFD-44D1-A4E3-0774FD0BAC15}" name="it"/>
-    <tableColumn id="5" xr3:uid="{3222D3A2-26F6-4B50-B423-C40487FE1EC4}" name="fr"/>
-    <tableColumn id="6" xr3:uid="{616BCBD8-3581-4F2F-9B1C-31ACE35035FE}" name="de"/>
-    <tableColumn id="7" xr3:uid="{9A002B4D-A4A3-4BEA-81E5-703F21AC9DC0}" name="nl"/>
-    <tableColumn id="8" xr3:uid="{B552B0B0-7C97-4F30-A9B3-F5664D12EED8}" name="ja"/>
-    <tableColumn id="9" xr3:uid="{1CE81ADD-EB4A-43B1-B848-8A2AFC0016C4}" name="fa"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D6DB3C6A-52AF-47F2-804D-582AA875016F}" name="Table2" displayName="Table2" ref="A1:I4" totalsRowShown="0">
   <autoFilter ref="A1:I4" xr:uid="{D6DB3C6A-52AF-47F2-804D-582AA875016F}"/>
   <tableColumns count="9">
@@ -2438,7 +2374,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7351F86F-FDC9-496A-8B76-65576F630D1F}" name="Table3" displayName="Table3" ref="A1:I7" totalsRowShown="0">
   <autoFilter ref="A1:I7" xr:uid="{7351F86F-FDC9-496A-8B76-65576F630D1F}"/>
   <tableColumns count="9">
@@ -2456,7 +2392,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DAC35E49-099B-4ABA-B147-F62078DC2770}" name="Table4" displayName="Table4" ref="A1:I5" totalsRowShown="0">
   <autoFilter ref="A1:I5" xr:uid="{DAC35E49-099B-4ABA-B147-F62078DC2770}"/>
   <tableColumns count="9">
@@ -2474,7 +2410,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0574641-9580-4C09-8594-7E1FA61261E7}" name="Table5" displayName="Table5" ref="A1:J2" totalsRowShown="0">
   <autoFilter ref="A1:J2" xr:uid="{D0574641-9580-4C09-8594-7E1FA61261E7}"/>
   <tableColumns count="10">
@@ -2493,7 +2429,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}" name="Table6" displayName="Table6" ref="A1:I85" totalsRowShown="0">
   <autoFilter ref="A1:I85" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}"/>
   <tableColumns count="9">
@@ -3027,7 +2963,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>714</v>
+        <v>698</v>
       </c>
       <c r="B12" t="s">
         <v>670</v>
@@ -3180,7 +3116,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>709</v>
+        <v>693</v>
       </c>
       <c r="B21" t="s">
         <v>668</v>
@@ -3205,122 +3141,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D3C9E3-8CD7-4EA8-BF66-BA0EEF0762E4}">
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>693</v>
-      </c>
-      <c r="B2" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>695</v>
-      </c>
-      <c r="B3" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>697</v>
-      </c>
-      <c r="B4" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
-        <v>699</v>
-      </c>
-      <c r="B5" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
-        <v>701</v>
-      </c>
-      <c r="B6" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
-        <v>703</v>
-      </c>
-      <c r="B7" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
-        <v>705</v>
-      </c>
-      <c r="B8" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
-        <v>707</v>
-      </c>
-      <c r="B9" t="s">
-        <v>708</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0971966-DEDD-44F5-9117-3B0FACFC4D1F}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3401,6 +3226,9 @@
       <c r="B4" t="s">
         <v>18</v>
       </c>
+      <c r="I4" t="s">
+        <v>732</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3410,7 +3238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FFD52D-082F-46A8-9C50-9791DEE86EEF}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -3642,7 +3470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7433A8F-1C59-4D32-A472-97E0718CFA1A}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -3769,7 +3597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E988A0-3272-4A07-B301-DE09586F293E}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -3854,11 +3682,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5C7B9E-E03D-420F-8955-42B4860CC822}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -4019,7 +3847,7 @@
         <v>104</v>
       </c>
       <c r="I5" t="s">
-        <v>712</v>
+        <v>696</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
@@ -4135,7 +3963,7 @@
         <v>129</v>
       </c>
       <c r="I9" t="s">
-        <v>710</v>
+        <v>694</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
@@ -4280,7 +4108,7 @@
         <v>162</v>
       </c>
       <c r="I14" t="s">
-        <v>711</v>
+        <v>695</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
@@ -4599,7 +4427,7 @@
         <v>227</v>
       </c>
       <c r="I25" t="s">
-        <v>713</v>
+        <v>697</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.5">
@@ -6199,147 +6027,147 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A81" t="s">
-        <v>743</v>
+        <v>727</v>
       </c>
       <c r="B81" t="s">
-        <v>715</v>
+        <v>699</v>
       </c>
       <c r="C81" t="s">
-        <v>716</v>
+        <v>700</v>
       </c>
       <c r="D81" t="s">
-        <v>717</v>
+        <v>701</v>
       </c>
       <c r="E81" t="s">
-        <v>718</v>
+        <v>702</v>
       </c>
       <c r="F81" t="s">
-        <v>719</v>
+        <v>703</v>
       </c>
       <c r="G81" t="s">
-        <v>720</v>
+        <v>704</v>
       </c>
       <c r="H81" t="s">
-        <v>721</v>
+        <v>705</v>
       </c>
       <c r="I81" t="s">
-        <v>722</v>
+        <v>706</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A82" t="s">
-        <v>744</v>
+        <v>728</v>
       </c>
       <c r="B82" t="s">
-        <v>723</v>
+        <v>707</v>
       </c>
       <c r="C82" t="s">
-        <v>724</v>
+        <v>708</v>
       </c>
       <c r="D82" t="s">
-        <v>725</v>
+        <v>709</v>
       </c>
       <c r="E82" t="s">
-        <v>723</v>
+        <v>707</v>
       </c>
       <c r="F82" t="s">
-        <v>726</v>
+        <v>710</v>
       </c>
       <c r="G82" t="s">
-        <v>727</v>
+        <v>711</v>
       </c>
       <c r="H82" t="s">
-        <v>728</v>
+        <v>712</v>
       </c>
       <c r="I82" t="s">
-        <v>729</v>
+        <v>713</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A83" t="s">
-        <v>745</v>
+        <v>729</v>
       </c>
       <c r="B83" t="s">
-        <v>730</v>
+        <v>714</v>
       </c>
       <c r="C83" t="s">
-        <v>730</v>
+        <v>714</v>
       </c>
       <c r="D83" t="s">
-        <v>730</v>
+        <v>714</v>
       </c>
       <c r="E83" t="s">
-        <v>731</v>
+        <v>715</v>
       </c>
       <c r="F83" t="s">
-        <v>732</v>
+        <v>716</v>
       </c>
       <c r="G83" t="s">
-        <v>730</v>
+        <v>714</v>
       </c>
       <c r="H83" t="s">
-        <v>733</v>
+        <v>717</v>
       </c>
       <c r="I83" t="s">
-        <v>734</v>
+        <v>718</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A84" t="s">
-        <v>746</v>
+        <v>730</v>
       </c>
       <c r="B84" t="s">
-        <v>735</v>
+        <v>719</v>
       </c>
       <c r="C84" t="s">
-        <v>736</v>
+        <v>720</v>
       </c>
       <c r="D84" t="s">
-        <v>735</v>
+        <v>719</v>
       </c>
       <c r="E84" t="s">
-        <v>737</v>
+        <v>721</v>
       </c>
       <c r="F84" t="s">
-        <v>735</v>
+        <v>719</v>
       </c>
       <c r="G84" t="s">
-        <v>737</v>
+        <v>721</v>
       </c>
       <c r="H84" t="s">
-        <v>738</v>
+        <v>722</v>
       </c>
       <c r="I84" t="s">
-        <v>739</v>
+        <v>723</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A85" t="s">
-        <v>747</v>
+        <v>731</v>
       </c>
       <c r="B85" t="s">
-        <v>740</v>
+        <v>724</v>
       </c>
       <c r="C85" t="s">
-        <v>740</v>
+        <v>724</v>
       </c>
       <c r="D85" t="s">
-        <v>740</v>
+        <v>724</v>
       </c>
       <c r="E85" t="s">
-        <v>740</v>
+        <v>724</v>
       </c>
       <c r="F85" t="s">
-        <v>740</v>
+        <v>724</v>
       </c>
       <c r="G85" t="s">
-        <v>740</v>
+        <v>724</v>
       </c>
       <c r="H85" t="s">
-        <v>741</v>
+        <v>725</v>
       </c>
       <c r="I85" t="s">
-        <v>742</v>
+        <v>726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added club teams for 2025 club world cup
</commit_message>
<xml_diff>
--- a/fonts/localization.xlsx
+++ b/fonts/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\fonts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/Documents/code/soccer-tourney-poster/fonts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFBA6FC-BE71-4A45-99E7-25A4899E395A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF39181-193A-4349-9CC6-3E481DA0B3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="19200" windowHeight="10073" activeTab="5" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="24660" windowHeight="15180" activeTab="6" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonts" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Group" sheetId="3" r:id="rId4"/>
     <sheet name="Match" sheetId="2" r:id="rId5"/>
     <sheet name="Team" sheetId="5" r:id="rId6"/>
+    <sheet name="Club" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="940">
   <si>
     <t>key</t>
   </si>
@@ -2324,12 +2325,561 @@
   <si>
     <t>jam</t>
   </si>
+  <si>
+    <t>Paris Saint-Germain</t>
+  </si>
+  <si>
+    <t>París Saint Germain</t>
+  </si>
+  <si>
+    <t>パリ・サンジェルマン</t>
+  </si>
+  <si>
+    <t>Atlético Madrid</t>
+  </si>
+  <si>
+    <t>Atlético de Madrid</t>
+  </si>
+  <si>
+    <t>Atletico Madrid</t>
+  </si>
+  <si>
+    <t>アトレティコ・マドリード</t>
+  </si>
+  <si>
+    <t>Botafogo</t>
+  </si>
+  <si>
+    <t>ボタフォゴ</t>
+  </si>
+  <si>
+    <t>Boca Juniors</t>
+  </si>
+  <si>
+    <t>Benfica</t>
+  </si>
+  <si>
+    <t>Espérance de Tunis</t>
+  </si>
+  <si>
+    <t>Esperanza de Túnez</t>
+  </si>
+  <si>
+    <t>Esperanza di Tunisi</t>
+  </si>
+  <si>
+    <t>エスペランス デ チュニス</t>
+  </si>
+  <si>
+    <t>Río de la Plata</t>
+  </si>
+  <si>
+    <t>Urawa Red Diamonds</t>
+  </si>
+  <si>
+    <t>Diamantes rojos de Urawa</t>
+  </si>
+  <si>
+    <t>Diamanti rossi Urawa</t>
+  </si>
+  <si>
+    <t>Diamants rouges d'Urawa</t>
+  </si>
+  <si>
+    <t>Rote Urawa-Diamanten</t>
+  </si>
+  <si>
+    <t>Urawa rode diamanten</t>
+  </si>
+  <si>
+    <t>浦和レッズ</t>
+  </si>
+  <si>
+    <t>Borussia Dortmund</t>
+  </si>
+  <si>
+    <t>ボルシア・ドルトムント</t>
+  </si>
+  <si>
+    <t>Manchester City</t>
+  </si>
+  <si>
+    <t>ciudad de manchester</t>
+  </si>
+  <si>
+    <t>Manchester-stad</t>
+  </si>
+  <si>
+    <t>マンチェスターシティ</t>
+  </si>
+  <si>
+    <t>Al Hilal</t>
+  </si>
+  <si>
+    <t>Al-Hilal</t>
+  </si>
+  <si>
+    <t>アル・ヒラル</t>
+  </si>
+  <si>
+    <t>پاری سن ژرمن</t>
+  </si>
+  <si>
+    <t>اتلتیکو مادرید</t>
+  </si>
+  <si>
+    <t>بوتافوگو</t>
+  </si>
+  <si>
+    <t>اسپرانس تونس</t>
+  </si>
+  <si>
+    <t>الماس قرمز اوراوا</t>
+  </si>
+  <si>
+    <t>بوروسیا دورتموند</t>
+  </si>
+  <si>
+    <t>منچستر سیتی</t>
+  </si>
+  <si>
+    <t>الهلال</t>
+  </si>
+  <si>
+    <t>pal</t>
+  </si>
+  <si>
+    <t>ahl</t>
+  </si>
+  <si>
+    <t>mia</t>
+  </si>
+  <si>
+    <t>psg</t>
+  </si>
+  <si>
+    <t>atm</t>
+  </si>
+  <si>
+    <t>bot</t>
+  </si>
+  <si>
+    <t>sea</t>
+  </si>
+  <si>
+    <t>bay</t>
+  </si>
+  <si>
+    <t>akl</t>
+  </si>
+  <si>
+    <t>boc</t>
+  </si>
+  <si>
+    <t>slb</t>
+  </si>
+  <si>
+    <t>fla</t>
+  </si>
+  <si>
+    <t>est</t>
+  </si>
+  <si>
+    <t>che</t>
+  </si>
+  <si>
+    <t>leo</t>
+  </si>
+  <si>
+    <t>riv</t>
+  </si>
+  <si>
+    <t>urd</t>
+  </si>
+  <si>
+    <t>cfm</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>flu</t>
+  </si>
+  <si>
+    <t>bvb</t>
+  </si>
+  <si>
+    <t>uhd</t>
+  </si>
+  <si>
+    <t>msu</t>
+  </si>
+  <si>
+    <t>mci</t>
+  </si>
+  <si>
+    <t>wac</t>
+  </si>
+  <si>
+    <t>ain</t>
+  </si>
+  <si>
+    <t>juv</t>
+  </si>
+  <si>
+    <t>rma</t>
+  </si>
+  <si>
+    <t>hil</t>
+  </si>
+  <si>
+    <t>pac</t>
+  </si>
+  <si>
+    <t>sal</t>
+  </si>
+  <si>
+    <t>Palmeiras</t>
+  </si>
+  <si>
+    <t>パルメイラス</t>
+  </si>
+  <si>
+    <t>پالمیراس</t>
+  </si>
+  <si>
+    <t>Porto</t>
+  </si>
+  <si>
+    <t>Oporto</t>
+  </si>
+  <si>
+    <t>ポルト</t>
+  </si>
+  <si>
+    <t>پورتو</t>
+  </si>
+  <si>
+    <t>Al Ahly</t>
+  </si>
+  <si>
+    <t>Al-Ahly</t>
+  </si>
+  <si>
+    <t>アル・アハリ</t>
+  </si>
+  <si>
+    <t>الاهلی</t>
+  </si>
+  <si>
+    <t>Inter Miami</t>
+  </si>
+  <si>
+    <t>InterMiami</t>
+  </si>
+  <si>
+    <t>インテル・マイアミ</t>
+  </si>
+  <si>
+    <t>اینتر میامی</t>
+  </si>
+  <si>
+    <t>Seattle Sounders</t>
+  </si>
+  <si>
+    <t>Sondas de Seattle</t>
+  </si>
+  <si>
+    <t>Sirene di Seattle</t>
+  </si>
+  <si>
+    <t>Sondeurs de Seattle</t>
+  </si>
+  <si>
+    <t>Seattle-sounders</t>
+  </si>
+  <si>
+    <t>シアトル・サウンダーズ</t>
+  </si>
+  <si>
+    <t>سیاتل ساندرز</t>
+  </si>
+  <si>
+    <t>Bayern Munich</t>
+  </si>
+  <si>
+    <t>Bayern de Múnich</t>
+  </si>
+  <si>
+    <t>Bayern Monaco</t>
+  </si>
+  <si>
+    <t>Bayern München</t>
+  </si>
+  <si>
+    <t>バイエルン・ミュンヘン</t>
+  </si>
+  <si>
+    <t>بایرن مونیخ</t>
+  </si>
+  <si>
+    <t>Auckland City</t>
+  </si>
+  <si>
+    <t>ciudad de auckland</t>
+  </si>
+  <si>
+    <t>Città di Auckland</t>
+  </si>
+  <si>
+    <t>Ville d'Auckland</t>
+  </si>
+  <si>
+    <t>Auckland-Stadt</t>
+  </si>
+  <si>
+    <t>Auckland stad</t>
+  </si>
+  <si>
+    <t>オークランド市</t>
+  </si>
+  <si>
+    <t>شهر اوکلند</t>
+  </si>
+  <si>
+    <t>Boca junioren</t>
+  </si>
+  <si>
+    <t>ボカ・ジュニアーズ</t>
+  </si>
+  <si>
+    <t>بوکا جونیورز</t>
+  </si>
+  <si>
+    <t>ベンフィカ</t>
+  </si>
+  <si>
+    <t>بنفیکا</t>
+  </si>
+  <si>
+    <t>Flamengo</t>
+  </si>
+  <si>
+    <t>flamenco</t>
+  </si>
+  <si>
+    <t>フラメンゴ</t>
+  </si>
+  <si>
+    <t>فلامنگو</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>チェルシー</t>
+  </si>
+  <si>
+    <t>چلسی</t>
+  </si>
+  <si>
+    <t>River Plate</t>
+  </si>
+  <si>
+    <t>Rivière Plate</t>
+  </si>
+  <si>
+    <t>Rivierplaat</t>
+  </si>
+  <si>
+    <t>リバープレート</t>
+  </si>
+  <si>
+    <t>ریور پلیت</t>
+  </si>
+  <si>
+    <t>Monterrey</t>
+  </si>
+  <si>
+    <t>モンテレー</t>
+  </si>
+  <si>
+    <t>مونتری</t>
+  </si>
+  <si>
+    <t>Inter Milan</t>
+  </si>
+  <si>
+    <t>Inter de Milán</t>
+  </si>
+  <si>
+    <t>Inter</t>
+  </si>
+  <si>
+    <t>Inter Mailand</t>
+  </si>
+  <si>
+    <t>Inter Milaan</t>
+  </si>
+  <si>
+    <t>インテル・ミラノ</t>
+  </si>
+  <si>
+    <t>اینترمیلان</t>
+  </si>
+  <si>
+    <t>Ulsan</t>
+  </si>
+  <si>
+    <t>蔚山</t>
+  </si>
+  <si>
+    <t>اولسان</t>
+  </si>
+  <si>
+    <t>Mamelodi Sundowns</t>
+  </si>
+  <si>
+    <t>Atardecer en Mamelodi</t>
+  </si>
+  <si>
+    <t>Tramonti Mamelodi</t>
+  </si>
+  <si>
+    <t>Couchers de soleil de Mamelodi</t>
+  </si>
+  <si>
+    <t>Mamelodi-Sonnenuntergänge</t>
+  </si>
+  <si>
+    <t>Mamelodi zonsondergangen</t>
+  </si>
+  <si>
+    <t>マメロディ サンダウンズ</t>
+  </si>
+  <si>
+    <t>Wydad</t>
+  </si>
+  <si>
+    <t>ウィダッド</t>
+  </si>
+  <si>
+    <t>ویداد</t>
+  </si>
+  <si>
+    <t>Al Ain</t>
+  </si>
+  <si>
+    <t>Al-Ain</t>
+  </si>
+  <si>
+    <t>Al-Aïn</t>
+  </si>
+  <si>
+    <t>アル・アイン</t>
+  </si>
+  <si>
+    <t>العین</t>
+  </si>
+  <si>
+    <t>Juventus</t>
+  </si>
+  <si>
+    <t>Juve</t>
+  </si>
+  <si>
+    <t>ユベントス</t>
+  </si>
+  <si>
+    <t>یوونتوس</t>
+  </si>
+  <si>
+    <t>Real Madrid</t>
+  </si>
+  <si>
+    <t>real madrid</t>
+  </si>
+  <si>
+    <t>Réal Madrid</t>
+  </si>
+  <si>
+    <t>Echt Madrid</t>
+  </si>
+  <si>
+    <t>レアル・マドリード</t>
+  </si>
+  <si>
+    <t>رئال مادرید</t>
+  </si>
+  <si>
+    <t>Pachuca</t>
+  </si>
+  <si>
+    <t>pachuca</t>
+  </si>
+  <si>
+    <t>パチューカ</t>
+  </si>
+  <si>
+    <t>پاچوکا</t>
+  </si>
+  <si>
+    <t>Salzburg</t>
+  </si>
+  <si>
+    <t>Salsburgo</t>
+  </si>
+  <si>
+    <t>Salisburgo</t>
+  </si>
+  <si>
+    <t>Salzbourg</t>
+  </si>
+  <si>
+    <t>Salzburgerland</t>
+  </si>
+  <si>
+    <t>ザルツブルク</t>
+  </si>
+  <si>
+    <t>سالزبورگ</t>
+  </si>
+  <si>
+    <t>Fluminense</t>
+  </si>
+  <si>
+    <t>fluminense</t>
+  </si>
+  <si>
+    <t>フルミネンセ</t>
+  </si>
+  <si>
+    <t>فلومیننس</t>
+  </si>
+  <si>
+    <t>León</t>
+  </si>
+  <si>
+    <t>Leone</t>
+  </si>
+  <si>
+    <t>Léon</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>レオン</t>
+  </si>
+  <si>
+    <t>لئون</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2349,6 +2899,20 @@
       <name val="MS Gothic"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2367,17 +2931,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2475,7 +3079,7 @@
     <tableColumn id="5" xr3:uid="{0318B88A-79B0-4BA8-931F-32E598CDDD83}" name="fr"/>
     <tableColumn id="6" xr3:uid="{7FB94F46-D9D6-4FFA-A68A-D9C22DD62960}" name="de"/>
     <tableColumn id="7" xr3:uid="{8DA7014B-3E29-4B6A-905E-FD5A34D770FA}" name="nl"/>
-    <tableColumn id="8" xr3:uid="{21D35627-DEB2-4E21-A7A7-5800DA843F2D}" name="ja" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{21D35627-DEB2-4E21-A7A7-5800DA843F2D}" name="ja" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{0E0ECA8B-5B6D-4A0F-9BA3-F5F697D5FD39}" name="fa"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2514,6 +3118,24 @@
     <tableColumn id="7" xr3:uid="{F6F798F3-5C50-4678-B680-669830CE2355}" name="nl"/>
     <tableColumn id="8" xr3:uid="{6C5220A1-9C59-4EE7-B606-9CDDB8959003}" name="ja"/>
     <tableColumn id="9" xr3:uid="{ABBFD51F-520B-4234-A795-3564F455A044}" name="fa"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}" name="Table8" displayName="Table8" ref="A1:I33" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="A1:I33" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{D098A691-2771-6641-BDA7-287210E02E79}" name="key" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{E3E8593F-CDB5-CA4C-B2DF-C5D167E6F581}" name="en"/>
+    <tableColumn id="3" xr3:uid="{583B6CFD-84CD-BB44-88B6-0A0D3BA2E05E}" name="es"/>
+    <tableColumn id="4" xr3:uid="{3139A9B8-E0C7-184A-8291-97B79E51FC05}" name="it"/>
+    <tableColumn id="5" xr3:uid="{FD4CA819-B010-2741-848E-AC69E248C01C}" name="fr"/>
+    <tableColumn id="6" xr3:uid="{EDBC100C-F7C3-E549-958D-AC9301A5B47B}" name="de"/>
+    <tableColumn id="7" xr3:uid="{15294C03-16B8-AF41-B968-8D069BF689CA}" name="nl"/>
+    <tableColumn id="8" xr3:uid="{A28E6B6D-690D-5C48-B30D-750602CBF93D}" name="ja"/>
+    <tableColumn id="9" xr3:uid="{AA78705B-5012-2C4D-8765-7F30AAFE5F05}" name="fa"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2822,16 +3444,16 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.9375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.87890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.87890625" customWidth="1"/>
-    <col min="9" max="9" width="11.9375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2863,7 +3485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>643</v>
       </c>
@@ -2880,7 +3502,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>644</v>
       </c>
@@ -2897,7 +3519,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>645</v>
       </c>
@@ -2914,7 +3536,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>646</v>
       </c>
@@ -2931,7 +3553,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>647</v>
       </c>
@@ -2948,7 +3570,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>648</v>
       </c>
@@ -2965,7 +3587,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>649</v>
       </c>
@@ -2982,7 +3604,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>650</v>
       </c>
@@ -2999,7 +3621,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>651</v>
       </c>
@@ -3016,7 +3638,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>652</v>
       </c>
@@ -3033,7 +3655,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>694</v>
       </c>
@@ -3050,7 +3672,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>653</v>
       </c>
@@ -3067,7 +3689,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>654</v>
       </c>
@@ -3084,7 +3706,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>655</v>
       </c>
@@ -3101,7 +3723,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>656</v>
       </c>
@@ -3118,7 +3740,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>657</v>
       </c>
@@ -3135,7 +3757,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>658</v>
       </c>
@@ -3152,7 +3774,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>659</v>
       </c>
@@ -3169,7 +3791,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>660</v>
       </c>
@@ -3186,7 +3808,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>689</v>
       </c>
@@ -3220,12 +3842,12 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3254,7 +3876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>640</v>
       </c>
@@ -3283,7 +3905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>641</v>
       </c>
@@ -3291,7 +3913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>642</v>
       </c>
@@ -3318,20 +3940,20 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.46875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.41015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.52734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.76171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5859375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.52734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.87890625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3360,7 +3982,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>635</v>
       </c>
@@ -3389,7 +4011,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>739</v>
       </c>
@@ -3418,7 +4040,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>740</v>
       </c>
@@ -3447,7 +4069,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>738</v>
       </c>
@@ -3476,7 +4098,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>636</v>
       </c>
@@ -3505,7 +4127,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>637</v>
       </c>
@@ -3534,7 +4156,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>638</v>
       </c>
@@ -3563,7 +4185,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>639</v>
       </c>
@@ -3608,12 +4230,12 @@
       <selection sqref="A1:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.64453125" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3642,7 +4264,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>685</v>
       </c>
@@ -3671,7 +4293,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>632</v>
       </c>
@@ -3697,7 +4319,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>633</v>
       </c>
@@ -3708,7 +4330,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>634</v>
       </c>
@@ -3735,12 +4357,12 @@
       <selection sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.9375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3772,7 +4394,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>631</v>
       </c>
@@ -3816,26 +4438,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5C7B9E-E03D-420F-8955-42B4860CC822}">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A66" sqref="A66"/>
+      <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.52734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.9375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.29296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.29296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.87890625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.29296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3864,7 +4486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>558</v>
       </c>
@@ -3893,7 +4515,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>559</v>
       </c>
@@ -3922,7 +4544,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>560</v>
       </c>
@@ -3951,7 +4573,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>561</v>
       </c>
@@ -3980,7 +4602,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>562</v>
       </c>
@@ -4009,7 +4631,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>563</v>
       </c>
@@ -4038,7 +4660,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>564</v>
       </c>
@@ -4067,7 +4689,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>565</v>
       </c>
@@ -4096,7 +4718,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>566</v>
       </c>
@@ -4125,7 +4747,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>567</v>
       </c>
@@ -4154,7 +4776,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>568</v>
       </c>
@@ -4183,7 +4805,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>569</v>
       </c>
@@ -4212,7 +4834,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>570</v>
       </c>
@@ -4241,7 +4863,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>571</v>
       </c>
@@ -4270,7 +4892,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>572</v>
       </c>
@@ -4299,7 +4921,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>573</v>
       </c>
@@ -4328,7 +4950,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>574</v>
       </c>
@@ -4357,7 +4979,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>575</v>
       </c>
@@ -4386,7 +5008,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>576</v>
       </c>
@@ -4415,7 +5037,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>577</v>
       </c>
@@ -4444,7 +5066,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>578</v>
       </c>
@@ -4473,7 +5095,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>579</v>
       </c>
@@ -4502,7 +5124,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>580</v>
       </c>
@@ -4531,7 +5153,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>581</v>
       </c>
@@ -4560,7 +5182,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>582</v>
       </c>
@@ -4589,7 +5211,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>583</v>
       </c>
@@ -4618,7 +5240,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>584</v>
       </c>
@@ -4647,7 +5269,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>585</v>
       </c>
@@ -4676,7 +5298,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>586</v>
       </c>
@@ -4705,7 +5327,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>587</v>
       </c>
@@ -4734,7 +5356,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>588</v>
       </c>
@@ -4763,7 +5385,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>589</v>
       </c>
@@ -4792,7 +5414,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>590</v>
       </c>
@@ -4821,7 +5443,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>731</v>
       </c>
@@ -4850,7 +5472,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>591</v>
       </c>
@@ -4879,7 +5501,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>592</v>
       </c>
@@ -4908,7 +5530,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>593</v>
       </c>
@@ -4937,7 +5559,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>594</v>
       </c>
@@ -4966,7 +5588,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>595</v>
       </c>
@@ -4995,7 +5617,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>596</v>
       </c>
@@ -5024,7 +5646,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>597</v>
       </c>
@@ -5053,7 +5675,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>598</v>
       </c>
@@ -5082,7 +5704,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>599</v>
       </c>
@@ -5111,7 +5733,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>600</v>
       </c>
@@ -5140,7 +5762,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>730</v>
       </c>
@@ -5169,7 +5791,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>601</v>
       </c>
@@ -5198,7 +5820,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>602</v>
       </c>
@@ -5227,7 +5849,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>603</v>
       </c>
@@ -5256,7 +5878,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>604</v>
       </c>
@@ -5285,7 +5907,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>605</v>
       </c>
@@ -5314,7 +5936,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>606</v>
       </c>
@@ -5343,7 +5965,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>607</v>
       </c>
@@ -5372,7 +5994,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>608</v>
       </c>
@@ -5401,7 +6023,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>609</v>
       </c>
@@ -5430,7 +6052,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>610</v>
       </c>
@@ -5459,7 +6081,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>611</v>
       </c>
@@ -5488,7 +6110,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>612</v>
       </c>
@@ -5517,7 +6139,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>613</v>
       </c>
@@ -5546,7 +6168,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>614</v>
       </c>
@@ -5575,7 +6197,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>615</v>
       </c>
@@ -5604,7 +6226,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>616</v>
       </c>
@@ -5633,7 +6255,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>617</v>
       </c>
@@ -5662,7 +6284,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>618</v>
       </c>
@@ -5691,7 +6313,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>756</v>
       </c>
@@ -5720,7 +6342,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>729</v>
       </c>
@@ -5749,7 +6371,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>619</v>
       </c>
@@ -5778,7 +6400,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>620</v>
       </c>
@@ -5807,7 +6429,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>621</v>
       </c>
@@ -5836,7 +6458,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>622</v>
       </c>
@@ -5865,7 +6487,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>623</v>
       </c>
@@ -5894,7 +6516,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>624</v>
       </c>
@@ -5923,7 +6545,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>625</v>
       </c>
@@ -5952,7 +6574,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>626</v>
       </c>
@@ -5981,7 +6603,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>585</v>
       </c>
@@ -6010,7 +6632,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>627</v>
       </c>
@@ -6039,7 +6661,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>628</v>
       </c>
@@ -6068,7 +6690,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>614</v>
       </c>
@@ -6097,7 +6719,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>629</v>
       </c>
@@ -6126,7 +6748,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>630</v>
       </c>
@@ -6155,7 +6777,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>723</v>
       </c>
@@ -6184,7 +6806,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>724</v>
       </c>
@@ -6213,7 +6835,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>725</v>
       </c>
@@ -6242,7 +6864,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>726</v>
       </c>
@@ -6271,7 +6893,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>727</v>
       </c>
@@ -6300,7 +6922,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>732</v>
       </c>
@@ -6335,4 +6957,992 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC23F0D-3FBD-1747-9B59-4A5AFE23CBEE}">
+  <dimension ref="A1:I33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>798</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>801</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>805</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>937</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>938</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>815</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>817</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>824</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>929</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A21" r:id="rId1" display="http://club.int/" xr:uid="{12F034EF-16B0-EE4E-8F2D-D0B9F820D947}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add LAFC to club list
</commit_message>
<xml_diff>
--- a/fonts/localization.xlsx
+++ b/fonts/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/Documents/code/soccer-tourney-poster/fonts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/fonts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF39181-193A-4349-9CC6-3E481DA0B3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7745040-53EA-D64E-9C72-181B77AF5C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="24660" windowHeight="15180" activeTab="6" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19760" activeTab="6" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonts" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="945">
   <si>
     <t>key</t>
   </si>
@@ -2873,6 +2873,21 @@
   </si>
   <si>
     <t>لئون</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Los Ángeles</t>
+  </si>
+  <si>
+    <t>ロサンゼルス</t>
+  </si>
+  <si>
+    <t>لس آنجلس</t>
+  </si>
+  <si>
+    <t>laf</t>
   </si>
 </sst>
 </file>
@@ -3124,8 +3139,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}" name="Table8" displayName="Table8" ref="A1:I33" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="A1:I33" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}" name="Table8" displayName="Table8" ref="A1:I34" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="A1:I34" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D098A691-2771-6641-BDA7-287210E02E79}" name="key" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{E3E8593F-CDB5-CA4C-B2DF-C5D167E6F581}" name="en"/>
@@ -6961,10 +6976,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC23F0D-3FBD-1747-9B59-4A5AFE23CBEE}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:I17"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7936,6 +7951,35 @@
         <v>929</v>
       </c>
     </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>944</v>
+      </c>
+      <c r="B34" t="s">
+        <v>940</v>
+      </c>
+      <c r="C34" t="s">
+        <v>941</v>
+      </c>
+      <c r="D34" t="s">
+        <v>940</v>
+      </c>
+      <c r="E34" t="s">
+        <v>940</v>
+      </c>
+      <c r="F34" t="s">
+        <v>940</v>
+      </c>
+      <c r="G34" t="s">
+        <v>940</v>
+      </c>
+      <c r="H34" t="s">
+        <v>942</v>
+      </c>
+      <c r="I34" t="s">
+        <v>943</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A21" r:id="rId1" display="http://club.int/" xr:uid="{12F034EF-16B0-EE4E-8F2D-D0B9F820D947}"/>

</xml_diff>

<commit_message>
'team' loc tab to 'country'; playoff "teams" in club/country lists.
</commit_message>
<xml_diff>
--- a/fonts/localization.xlsx
+++ b/fonts/localization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/fonts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7745040-53EA-D64E-9C72-181B77AF5C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F233B456-23B3-8E4D-90AE-D1BE0F4A43FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19760" activeTab="6" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19740" activeTab="5" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonts" sheetId="6" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="Stage" sheetId="4" r:id="rId3"/>
     <sheet name="Group" sheetId="3" r:id="rId4"/>
     <sheet name="Match" sheetId="2" r:id="rId5"/>
-    <sheet name="Team" sheetId="5" r:id="rId6"/>
+    <sheet name="Country" sheetId="5" r:id="rId6"/>
     <sheet name="Club" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="993">
   <si>
     <t>key</t>
   </si>
@@ -2888,6 +2887,150 @@
   </si>
   <si>
     <t>laf</t>
+  </si>
+  <si>
+    <t>Play-Off A</t>
+  </si>
+  <si>
+    <t>Repechaje A</t>
+  </si>
+  <si>
+    <t>Barrage A</t>
+  </si>
+  <si>
+    <t>プレーオフ A</t>
+  </si>
+  <si>
+    <t>پلی‌آف A</t>
+  </si>
+  <si>
+    <t>Play-Off B</t>
+  </si>
+  <si>
+    <t>Repechaje B</t>
+  </si>
+  <si>
+    <t>Barrage B</t>
+  </si>
+  <si>
+    <t>プレーオフ B</t>
+  </si>
+  <si>
+    <t>پلی‌آف B</t>
+  </si>
+  <si>
+    <t>Play-Off C</t>
+  </si>
+  <si>
+    <t>Repechaje C</t>
+  </si>
+  <si>
+    <t>Barrage C</t>
+  </si>
+  <si>
+    <t>プレーオフ C</t>
+  </si>
+  <si>
+    <t>پلی‌آف C</t>
+  </si>
+  <si>
+    <t>Play-Off D</t>
+  </si>
+  <si>
+    <t>Repechaje D</t>
+  </si>
+  <si>
+    <t>Barrage D</t>
+  </si>
+  <si>
+    <t>プレーオフ D</t>
+  </si>
+  <si>
+    <t>پلی‌آف D</t>
+  </si>
+  <si>
+    <t>Play-Off 1</t>
+  </si>
+  <si>
+    <t>Repechaje 1</t>
+  </si>
+  <si>
+    <t>Barrage 1</t>
+  </si>
+  <si>
+    <t>プレーオフ 1</t>
+  </si>
+  <si>
+    <t>پلی‌آف 1</t>
+  </si>
+  <si>
+    <t>Play-Off 2</t>
+  </si>
+  <si>
+    <t>Repechaje 2</t>
+  </si>
+  <si>
+    <t>Barrage 2</t>
+  </si>
+  <si>
+    <t>プレーオフ 2</t>
+  </si>
+  <si>
+    <t>پلی‌آف 2</t>
+  </si>
+  <si>
+    <t>Play-Off 3</t>
+  </si>
+  <si>
+    <t>Repechaje 3</t>
+  </si>
+  <si>
+    <t>Barrage 3</t>
+  </si>
+  <si>
+    <t>プレーオフ 3</t>
+  </si>
+  <si>
+    <t>پلی‌آف 3</t>
+  </si>
+  <si>
+    <t>Play-Off 4</t>
+  </si>
+  <si>
+    <t>Repechaje 4</t>
+  </si>
+  <si>
+    <t>Barrage 4</t>
+  </si>
+  <si>
+    <t>プレーオフ 4</t>
+  </si>
+  <si>
+    <t>پلی‌آف 4</t>
+  </si>
+  <si>
+    <t>??A</t>
+  </si>
+  <si>
+    <t>??B</t>
+  </si>
+  <si>
+    <t>??C</t>
+  </si>
+  <si>
+    <t>??D</t>
+  </si>
+  <si>
+    <t>??1</t>
+  </si>
+  <si>
+    <t>??2</t>
+  </si>
+  <si>
+    <t>??3</t>
+  </si>
+  <si>
+    <t>??4</t>
   </si>
 </sst>
 </file>
@@ -3121,8 +3264,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}" name="Table6" displayName="Table6" ref="A1:I86" totalsRowShown="0">
-  <autoFilter ref="A1:I86" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}" name="Table6" displayName="Table6" ref="A1:I94" totalsRowShown="0">
+  <autoFilter ref="A1:I94" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2E55F9A9-3EF2-4534-84B5-0331227CCA52}" name="key"/>
     <tableColumn id="2" xr3:uid="{AAAAE7A0-7BF8-498D-8AB7-8D288BC7367E}" name="en"/>
@@ -3139,8 +3282,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}" name="Table8" displayName="Table8" ref="A1:I34" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="A1:I34" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}" name="Table8" displayName="Table8" ref="A1:I42" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="A1:I42" xr:uid="{BA8C5955-F911-B84D-96F6-FB2E611CA222}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D098A691-2771-6641-BDA7-287210E02E79}" name="key" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{E3E8593F-CDB5-CA4C-B2DF-C5D167E6F581}" name="en"/>
@@ -4451,13 +4594,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5C7B9E-E03D-420F-8955-42B4860CC822}">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="A87" sqref="A87:I94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6966,6 +7109,238 @@
         <v>737</v>
       </c>
     </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>985</v>
+      </c>
+      <c r="B87" t="s">
+        <v>945</v>
+      </c>
+      <c r="C87" t="s">
+        <v>946</v>
+      </c>
+      <c r="D87" t="s">
+        <v>945</v>
+      </c>
+      <c r="E87" t="s">
+        <v>947</v>
+      </c>
+      <c r="F87" t="s">
+        <v>945</v>
+      </c>
+      <c r="G87" t="s">
+        <v>945</v>
+      </c>
+      <c r="H87" t="s">
+        <v>948</v>
+      </c>
+      <c r="I87" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>986</v>
+      </c>
+      <c r="B88" t="s">
+        <v>950</v>
+      </c>
+      <c r="C88" t="s">
+        <v>951</v>
+      </c>
+      <c r="D88" t="s">
+        <v>950</v>
+      </c>
+      <c r="E88" t="s">
+        <v>952</v>
+      </c>
+      <c r="F88" t="s">
+        <v>950</v>
+      </c>
+      <c r="G88" t="s">
+        <v>950</v>
+      </c>
+      <c r="H88" t="s">
+        <v>953</v>
+      </c>
+      <c r="I88" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>987</v>
+      </c>
+      <c r="B89" t="s">
+        <v>955</v>
+      </c>
+      <c r="C89" t="s">
+        <v>956</v>
+      </c>
+      <c r="D89" t="s">
+        <v>955</v>
+      </c>
+      <c r="E89" t="s">
+        <v>957</v>
+      </c>
+      <c r="F89" t="s">
+        <v>955</v>
+      </c>
+      <c r="G89" t="s">
+        <v>955</v>
+      </c>
+      <c r="H89" t="s">
+        <v>958</v>
+      </c>
+      <c r="I89" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>988</v>
+      </c>
+      <c r="B90" t="s">
+        <v>960</v>
+      </c>
+      <c r="C90" t="s">
+        <v>961</v>
+      </c>
+      <c r="D90" t="s">
+        <v>960</v>
+      </c>
+      <c r="E90" t="s">
+        <v>962</v>
+      </c>
+      <c r="F90" t="s">
+        <v>960</v>
+      </c>
+      <c r="G90" t="s">
+        <v>960</v>
+      </c>
+      <c r="H90" t="s">
+        <v>963</v>
+      </c>
+      <c r="I90" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>989</v>
+      </c>
+      <c r="B91" t="s">
+        <v>965</v>
+      </c>
+      <c r="C91" t="s">
+        <v>966</v>
+      </c>
+      <c r="D91" t="s">
+        <v>965</v>
+      </c>
+      <c r="E91" t="s">
+        <v>967</v>
+      </c>
+      <c r="F91" t="s">
+        <v>965</v>
+      </c>
+      <c r="G91" t="s">
+        <v>965</v>
+      </c>
+      <c r="H91" t="s">
+        <v>968</v>
+      </c>
+      <c r="I91" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>990</v>
+      </c>
+      <c r="B92" t="s">
+        <v>970</v>
+      </c>
+      <c r="C92" t="s">
+        <v>971</v>
+      </c>
+      <c r="D92" t="s">
+        <v>970</v>
+      </c>
+      <c r="E92" t="s">
+        <v>972</v>
+      </c>
+      <c r="F92" t="s">
+        <v>970</v>
+      </c>
+      <c r="G92" t="s">
+        <v>970</v>
+      </c>
+      <c r="H92" t="s">
+        <v>973</v>
+      </c>
+      <c r="I92" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>991</v>
+      </c>
+      <c r="B93" t="s">
+        <v>975</v>
+      </c>
+      <c r="C93" t="s">
+        <v>976</v>
+      </c>
+      <c r="D93" t="s">
+        <v>975</v>
+      </c>
+      <c r="E93" t="s">
+        <v>977</v>
+      </c>
+      <c r="F93" t="s">
+        <v>975</v>
+      </c>
+      <c r="G93" t="s">
+        <v>975</v>
+      </c>
+      <c r="H93" t="s">
+        <v>978</v>
+      </c>
+      <c r="I93" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>992</v>
+      </c>
+      <c r="B94" t="s">
+        <v>980</v>
+      </c>
+      <c r="C94" t="s">
+        <v>981</v>
+      </c>
+      <c r="D94" t="s">
+        <v>980</v>
+      </c>
+      <c r="E94" t="s">
+        <v>982</v>
+      </c>
+      <c r="F94" t="s">
+        <v>980</v>
+      </c>
+      <c r="G94" t="s">
+        <v>980</v>
+      </c>
+      <c r="H94" t="s">
+        <v>983</v>
+      </c>
+      <c r="I94" t="s">
+        <v>984</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -6976,10 +7351,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC23F0D-3FBD-1747-9B59-4A5AFE23CBEE}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A10" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7980,6 +8355,238 @@
         <v>943</v>
       </c>
     </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="B35" t="s">
+        <v>945</v>
+      </c>
+      <c r="C35" t="s">
+        <v>946</v>
+      </c>
+      <c r="D35" t="s">
+        <v>945</v>
+      </c>
+      <c r="E35" t="s">
+        <v>947</v>
+      </c>
+      <c r="F35" t="s">
+        <v>945</v>
+      </c>
+      <c r="G35" t="s">
+        <v>945</v>
+      </c>
+      <c r="H35" t="s">
+        <v>948</v>
+      </c>
+      <c r="I35" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="B36" t="s">
+        <v>950</v>
+      </c>
+      <c r="C36" t="s">
+        <v>951</v>
+      </c>
+      <c r="D36" t="s">
+        <v>950</v>
+      </c>
+      <c r="E36" t="s">
+        <v>952</v>
+      </c>
+      <c r="F36" t="s">
+        <v>950</v>
+      </c>
+      <c r="G36" t="s">
+        <v>950</v>
+      </c>
+      <c r="H36" t="s">
+        <v>953</v>
+      </c>
+      <c r="I36" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="B37" t="s">
+        <v>955</v>
+      </c>
+      <c r="C37" t="s">
+        <v>956</v>
+      </c>
+      <c r="D37" t="s">
+        <v>955</v>
+      </c>
+      <c r="E37" t="s">
+        <v>957</v>
+      </c>
+      <c r="F37" t="s">
+        <v>955</v>
+      </c>
+      <c r="G37" t="s">
+        <v>955</v>
+      </c>
+      <c r="H37" t="s">
+        <v>958</v>
+      </c>
+      <c r="I37" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B38" t="s">
+        <v>960</v>
+      </c>
+      <c r="C38" t="s">
+        <v>961</v>
+      </c>
+      <c r="D38" t="s">
+        <v>960</v>
+      </c>
+      <c r="E38" t="s">
+        <v>962</v>
+      </c>
+      <c r="F38" t="s">
+        <v>960</v>
+      </c>
+      <c r="G38" t="s">
+        <v>960</v>
+      </c>
+      <c r="H38" t="s">
+        <v>963</v>
+      </c>
+      <c r="I38" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="B39" t="s">
+        <v>965</v>
+      </c>
+      <c r="C39" t="s">
+        <v>966</v>
+      </c>
+      <c r="D39" t="s">
+        <v>965</v>
+      </c>
+      <c r="E39" t="s">
+        <v>967</v>
+      </c>
+      <c r="F39" t="s">
+        <v>965</v>
+      </c>
+      <c r="G39" t="s">
+        <v>965</v>
+      </c>
+      <c r="H39" t="s">
+        <v>968</v>
+      </c>
+      <c r="I39" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>990</v>
+      </c>
+      <c r="B40" t="s">
+        <v>970</v>
+      </c>
+      <c r="C40" t="s">
+        <v>971</v>
+      </c>
+      <c r="D40" t="s">
+        <v>970</v>
+      </c>
+      <c r="E40" t="s">
+        <v>972</v>
+      </c>
+      <c r="F40" t="s">
+        <v>970</v>
+      </c>
+      <c r="G40" t="s">
+        <v>970</v>
+      </c>
+      <c r="H40" t="s">
+        <v>973</v>
+      </c>
+      <c r="I40" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>991</v>
+      </c>
+      <c r="B41" t="s">
+        <v>975</v>
+      </c>
+      <c r="C41" t="s">
+        <v>976</v>
+      </c>
+      <c r="D41" t="s">
+        <v>975</v>
+      </c>
+      <c r="E41" t="s">
+        <v>977</v>
+      </c>
+      <c r="F41" t="s">
+        <v>975</v>
+      </c>
+      <c r="G41" t="s">
+        <v>975</v>
+      </c>
+      <c r="H41" t="s">
+        <v>978</v>
+      </c>
+      <c r="I41" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>992</v>
+      </c>
+      <c r="B42" t="s">
+        <v>980</v>
+      </c>
+      <c r="C42" t="s">
+        <v>981</v>
+      </c>
+      <c r="D42" t="s">
+        <v>980</v>
+      </c>
+      <c r="E42" t="s">
+        <v>982</v>
+      </c>
+      <c r="F42" t="s">
+        <v>980</v>
+      </c>
+      <c r="G42" t="s">
+        <v>980</v>
+      </c>
+      <c r="H42" t="s">
+        <v>983</v>
+      </c>
+      <c r="I42" t="s">
+        <v>984</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A21" r:id="rId1" display="http://club.int/" xr:uid="{12F034EF-16B0-EE4E-8F2D-D0B9F820D947}"/>

</xml_diff>

<commit_message>
2026 WC pre-playoff seedings
</commit_message>
<xml_diff>
--- a/fonts/localization.xlsx
+++ b/fonts/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/fonts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F233B456-23B3-8E4D-90AE-D1BE0F4A43FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8598DB-751A-014B-9C1F-A2788650DE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19740" activeTab="5" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="10100" yWindow="700" windowWidth="10020" windowHeight="19740" activeTab="5" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonts" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Country" sheetId="5" r:id="rId6"/>
     <sheet name="Club" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,6 +33,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="1025">
   <si>
     <t>key</t>
   </si>
@@ -3031,6 +3032,102 @@
   </si>
   <si>
     <t>??4</t>
+  </si>
+  <si>
+    <t>Curaçao</t>
+  </si>
+  <si>
+    <t>Curazao</t>
+  </si>
+  <si>
+    <t>Curacao</t>
+  </si>
+  <si>
+    <t>キュラソー</t>
+  </si>
+  <si>
+    <t>کوراسائو</t>
+  </si>
+  <si>
+    <t>cuw</t>
+  </si>
+  <si>
+    <t>civ</t>
+  </si>
+  <si>
+    <t>cpv</t>
+  </si>
+  <si>
+    <t>Cabo Verde</t>
+  </si>
+  <si>
+    <t>Capo Verde</t>
+  </si>
+  <si>
+    <t>Cap-Vert</t>
+  </si>
+  <si>
+    <t>Kap Verde</t>
+  </si>
+  <si>
+    <t>Kaapverdië</t>
+  </si>
+  <si>
+    <t>カーボベルデ</t>
+  </si>
+  <si>
+    <t>کیپ ورد</t>
+  </si>
+  <si>
+    <t>jor</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Jordán</t>
+  </si>
+  <si>
+    <t>Giordania</t>
+  </si>
+  <si>
+    <t>Jordanie</t>
+  </si>
+  <si>
+    <t>Jordanien</t>
+  </si>
+  <si>
+    <t>Jordanië</t>
+  </si>
+  <si>
+    <t>ヨルダン</t>
+  </si>
+  <si>
+    <t>اردن</t>
+  </si>
+  <si>
+    <t>uzb</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Uzbekistán</t>
+  </si>
+  <si>
+    <t>Ouzbékistan</t>
+  </si>
+  <si>
+    <t>Usbekistan</t>
+  </si>
+  <si>
+    <t>Oezbekistan</t>
+  </si>
+  <si>
+    <t>ウズベキスタン</t>
+  </si>
+  <si>
+    <t>ازبکستان</t>
   </si>
 </sst>
 </file>
@@ -3264,8 +3361,11 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}" name="Table6" displayName="Table6" ref="A1:I94" totalsRowShown="0">
-  <autoFilter ref="A1:I94" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}" name="Table6" displayName="Table6" ref="A1:I99" totalsRowShown="0">
+  <autoFilter ref="A1:I99" xr:uid="{1B6050B0-65A6-4FEE-8DCA-04DFBBE79E70}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I99">
+    <sortCondition ref="A1:A99"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2E55F9A9-3EF2-4534-84B5-0331227CCA52}" name="key"/>
     <tableColumn id="2" xr3:uid="{AAAAE7A0-7BF8-498D-8AB7-8D288BC7367E}" name="en"/>
@@ -4594,13 +4694,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5C7B9E-E03D-420F-8955-42B4860CC822}">
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A87" sqref="A87:I94"/>
+      <selection pane="bottomRight" activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4646,872 +4746,872 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>558</v>
+        <v>989</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>965</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>966</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>965</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>967</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>965</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>965</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>968</v>
       </c>
       <c r="I2" t="s">
-        <v>85</v>
+        <v>969</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>559</v>
+        <v>990</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>970</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>971</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>970</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>972</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>970</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>970</v>
       </c>
       <c r="H3" t="s">
-        <v>92</v>
+        <v>973</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>974</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>560</v>
+        <v>991</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>975</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>976</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>975</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>977</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>975</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>975</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>978</v>
       </c>
       <c r="I4" t="s">
-        <v>99</v>
+        <v>979</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>561</v>
+        <v>992</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>980</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>981</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>980</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>982</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>980</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
+        <v>980</v>
       </c>
       <c r="H5" t="s">
-        <v>104</v>
+        <v>983</v>
       </c>
       <c r="I5" t="s">
-        <v>692</v>
+        <v>984</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>562</v>
+        <v>985</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>945</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>946</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>945</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>947</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>945</v>
       </c>
       <c r="G6" t="s">
-        <v>109</v>
+        <v>945</v>
       </c>
       <c r="H6" t="s">
-        <v>110</v>
+        <v>948</v>
       </c>
       <c r="I6" t="s">
-        <v>111</v>
+        <v>949</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>563</v>
+        <v>986</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>950</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>951</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>950</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>952</v>
       </c>
       <c r="F7" t="s">
-        <v>115</v>
+        <v>950</v>
       </c>
       <c r="G7" t="s">
-        <v>116</v>
+        <v>950</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
+        <v>953</v>
       </c>
       <c r="I7" t="s">
-        <v>118</v>
+        <v>954</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>564</v>
+        <v>987</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>955</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>956</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>955</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>957</v>
       </c>
       <c r="F8" t="s">
-        <v>123</v>
+        <v>955</v>
       </c>
       <c r="G8" t="s">
-        <v>124</v>
+        <v>955</v>
       </c>
       <c r="H8" t="s">
-        <v>125</v>
+        <v>958</v>
       </c>
       <c r="I8" t="s">
-        <v>126</v>
+        <v>959</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>565</v>
+        <v>988</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>960</v>
       </c>
       <c r="C9" t="s">
-        <v>127</v>
+        <v>961</v>
       </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>960</v>
       </c>
       <c r="E9" t="s">
-        <v>127</v>
+        <v>962</v>
       </c>
       <c r="F9" t="s">
-        <v>127</v>
+        <v>960</v>
       </c>
       <c r="G9" t="s">
-        <v>127</v>
+        <v>960</v>
       </c>
       <c r="H9" t="s">
-        <v>129</v>
+        <v>963</v>
       </c>
       <c r="I9" t="s">
-        <v>690</v>
+        <v>964</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>566</v>
+        <v>619</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>480</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>480</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>480</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>481</v>
       </c>
       <c r="F10" t="s">
-        <v>134</v>
+        <v>482</v>
       </c>
       <c r="G10" t="s">
-        <v>130</v>
+        <v>483</v>
       </c>
       <c r="H10" t="s">
-        <v>135</v>
+        <v>484</v>
       </c>
       <c r="I10" t="s">
-        <v>136</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>567</v>
+        <v>600</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>351</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>352</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>351</v>
       </c>
       <c r="E11" t="s">
-        <v>140</v>
+        <v>353</v>
       </c>
       <c r="F11" t="s">
-        <v>141</v>
+        <v>354</v>
       </c>
       <c r="G11" t="s">
-        <v>142</v>
+        <v>355</v>
       </c>
       <c r="H11" t="s">
-        <v>143</v>
+        <v>356</v>
       </c>
       <c r="I11" t="s">
-        <v>144</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="F12" t="s">
-        <v>149</v>
+        <v>102</v>
       </c>
       <c r="G12" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="H12" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="I12" t="s">
-        <v>152</v>
+        <v>692</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>569</v>
+        <v>629</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>544</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>544</v>
       </c>
       <c r="D13" t="s">
-        <v>155</v>
+        <v>544</v>
       </c>
       <c r="E13" t="s">
-        <v>156</v>
+        <v>545</v>
       </c>
       <c r="F13" t="s">
-        <v>157</v>
+        <v>546</v>
       </c>
       <c r="G13" t="s">
-        <v>158</v>
+        <v>547</v>
       </c>
       <c r="H13" t="s">
-        <v>159</v>
+        <v>548</v>
       </c>
       <c r="I13" t="s">
-        <v>160</v>
+        <v>549</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>570</v>
+        <v>598</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>337</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>337</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>337</v>
       </c>
       <c r="E14" t="s">
-        <v>161</v>
+        <v>338</v>
       </c>
       <c r="F14" t="s">
-        <v>161</v>
+        <v>339</v>
       </c>
       <c r="G14" t="s">
-        <v>161</v>
+        <v>340</v>
       </c>
       <c r="H14" t="s">
-        <v>162</v>
+        <v>341</v>
       </c>
       <c r="I14" t="s">
-        <v>691</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>571</v>
+        <v>731</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>280</v>
       </c>
       <c r="C15" t="s">
-        <v>164</v>
+        <v>280</v>
       </c>
       <c r="D15" t="s">
-        <v>165</v>
+        <v>280</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
+        <v>281</v>
       </c>
       <c r="F15" t="s">
-        <v>167</v>
+        <v>282</v>
       </c>
       <c r="G15" t="s">
-        <v>168</v>
+        <v>283</v>
       </c>
       <c r="H15" t="s">
-        <v>169</v>
+        <v>284</v>
       </c>
       <c r="I15" t="s">
-        <v>170</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>572</v>
+        <v>614</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>436</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>437</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>438</v>
       </c>
       <c r="E16" t="s">
-        <v>171</v>
+        <v>439</v>
       </c>
       <c r="F16" t="s">
-        <v>171</v>
+        <v>440</v>
       </c>
       <c r="G16" t="s">
-        <v>171</v>
+        <v>441</v>
       </c>
       <c r="H16" t="s">
-        <v>173</v>
+        <v>442</v>
       </c>
       <c r="I16" t="s">
-        <v>174</v>
+        <v>443</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>573</v>
+        <v>614</v>
       </c>
       <c r="B17" t="s">
-        <v>175</v>
+        <v>539</v>
       </c>
       <c r="C17" t="s">
-        <v>176</v>
+        <v>540</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>539</v>
       </c>
       <c r="E17" t="s">
-        <v>178</v>
+        <v>541</v>
       </c>
       <c r="F17" t="s">
-        <v>179</v>
+        <v>539</v>
       </c>
       <c r="G17" t="s">
-        <v>180</v>
+        <v>540</v>
       </c>
       <c r="H17" t="s">
-        <v>181</v>
+        <v>542</v>
       </c>
       <c r="I17" t="s">
-        <v>182</v>
+        <v>543</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>574</v>
+        <v>559</v>
       </c>
       <c r="B18" t="s">
-        <v>183</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
-        <v>183</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>183</v>
+        <v>88</v>
       </c>
       <c r="E18" t="s">
-        <v>184</v>
+        <v>89</v>
       </c>
       <c r="F18" t="s">
-        <v>185</v>
+        <v>90</v>
       </c>
       <c r="G18" t="s">
-        <v>183</v>
+        <v>91</v>
       </c>
       <c r="H18" t="s">
-        <v>186</v>
+        <v>92</v>
       </c>
       <c r="I18" t="s">
-        <v>187</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>575</v>
+        <v>611</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>424</v>
       </c>
       <c r="C19" t="s">
-        <v>189</v>
+        <v>424</v>
       </c>
       <c r="D19" t="s">
-        <v>190</v>
+        <v>424</v>
       </c>
       <c r="E19" t="s">
-        <v>191</v>
+        <v>424</v>
       </c>
       <c r="F19" t="s">
-        <v>188</v>
+        <v>424</v>
       </c>
       <c r="G19" t="s">
-        <v>188</v>
+        <v>424</v>
       </c>
       <c r="H19" t="s">
-        <v>192</v>
+        <v>425</v>
       </c>
       <c r="I19" t="s">
-        <v>193</v>
+        <v>426</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>576</v>
+        <v>630</v>
       </c>
       <c r="B20" t="s">
-        <v>194</v>
+        <v>550</v>
       </c>
       <c r="C20" t="s">
-        <v>195</v>
+        <v>551</v>
       </c>
       <c r="D20" t="s">
-        <v>196</v>
+        <v>552</v>
       </c>
       <c r="E20" t="s">
-        <v>197</v>
+        <v>553</v>
       </c>
       <c r="F20" t="s">
-        <v>198</v>
+        <v>554</v>
       </c>
       <c r="G20" t="s">
-        <v>199</v>
+        <v>555</v>
       </c>
       <c r="H20" t="s">
-        <v>200</v>
+        <v>556</v>
       </c>
       <c r="I20" t="s">
-        <v>201</v>
+        <v>557</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>577</v>
+        <v>627</v>
       </c>
       <c r="B21" t="s">
-        <v>202</v>
+        <v>530</v>
       </c>
       <c r="C21" t="s">
-        <v>202</v>
+        <v>530</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
+        <v>530</v>
       </c>
       <c r="E21" t="s">
-        <v>203</v>
+        <v>531</v>
       </c>
       <c r="F21" t="s">
-        <v>202</v>
+        <v>532</v>
       </c>
       <c r="G21" t="s">
-        <v>202</v>
+        <v>533</v>
       </c>
       <c r="H21" t="s">
-        <v>204</v>
+        <v>534</v>
       </c>
       <c r="I21" t="s">
-        <v>205</v>
+        <v>535</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>578</v>
+        <v>558</v>
       </c>
       <c r="B22" t="s">
-        <v>206</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>206</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
+        <v>80</v>
       </c>
       <c r="E22" t="s">
-        <v>207</v>
+        <v>81</v>
       </c>
       <c r="F22" t="s">
-        <v>206</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s">
-        <v>206</v>
+        <v>83</v>
       </c>
       <c r="H22" t="s">
-        <v>208</v>
+        <v>84</v>
       </c>
       <c r="I22" t="s">
-        <v>209</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>579</v>
+        <v>625</v>
       </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>514</v>
       </c>
       <c r="C23" t="s">
-        <v>211</v>
+        <v>514</v>
       </c>
       <c r="D23" t="s">
-        <v>212</v>
+        <v>514</v>
       </c>
       <c r="E23" t="s">
-        <v>213</v>
+        <v>515</v>
       </c>
       <c r="F23" t="s">
-        <v>210</v>
+        <v>516</v>
       </c>
       <c r="G23" t="s">
-        <v>210</v>
+        <v>517</v>
       </c>
       <c r="H23" t="s">
-        <v>214</v>
+        <v>518</v>
       </c>
       <c r="I23" t="s">
-        <v>215</v>
+        <v>519</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>580</v>
+        <v>594</v>
       </c>
       <c r="B24" t="s">
-        <v>216</v>
+        <v>308</v>
       </c>
       <c r="C24" t="s">
-        <v>217</v>
+        <v>309</v>
       </c>
       <c r="D24" t="s">
-        <v>218</v>
+        <v>308</v>
       </c>
       <c r="E24" t="s">
-        <v>219</v>
+        <v>308</v>
       </c>
       <c r="F24" t="s">
-        <v>216</v>
+        <v>310</v>
       </c>
       <c r="G24" t="s">
-        <v>216</v>
+        <v>308</v>
       </c>
       <c r="H24" t="s">
-        <v>220</v>
+        <v>311</v>
       </c>
       <c r="I24" t="s">
-        <v>221</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="B25" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="C25" t="s">
-        <v>223</v>
+        <v>246</v>
       </c>
       <c r="D25" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="E25" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="F25" t="s">
-        <v>226</v>
+        <v>246</v>
       </c>
       <c r="G25" t="s">
-        <v>226</v>
+        <v>248</v>
       </c>
       <c r="H25" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="I25" t="s">
-        <v>693</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="B26" t="s">
-        <v>228</v>
+        <v>525</v>
       </c>
       <c r="C26" t="s">
-        <v>228</v>
+        <v>525</v>
       </c>
       <c r="D26" t="s">
-        <v>228</v>
+        <v>526</v>
       </c>
       <c r="E26" t="s">
-        <v>229</v>
+        <v>527</v>
       </c>
       <c r="F26" t="s">
-        <v>230</v>
+        <v>525</v>
       </c>
       <c r="G26" t="s">
-        <v>231</v>
+        <v>525</v>
       </c>
       <c r="H26" t="s">
-        <v>232</v>
+        <v>528</v>
       </c>
       <c r="I26" t="s">
-        <v>233</v>
+        <v>529</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>583</v>
+        <v>999</v>
       </c>
       <c r="B27" t="s">
-        <v>234</v>
+        <v>404</v>
       </c>
       <c r="C27" t="s">
-        <v>235</v>
+        <v>402</v>
       </c>
       <c r="D27" t="s">
-        <v>235</v>
+        <v>403</v>
       </c>
       <c r="E27" t="s">
-        <v>236</v>
+        <v>404</v>
       </c>
       <c r="F27" t="s">
-        <v>237</v>
+        <v>405</v>
       </c>
       <c r="G27" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="H27" t="s">
-        <v>238</v>
+        <v>407</v>
       </c>
       <c r="I27" t="s">
-        <v>239</v>
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>584</v>
+        <v>593</v>
       </c>
       <c r="B28" t="s">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="C28" t="s">
-        <v>241</v>
+        <v>301</v>
       </c>
       <c r="D28" t="s">
-        <v>242</v>
+        <v>302</v>
       </c>
       <c r="E28" t="s">
-        <v>240</v>
+        <v>303</v>
       </c>
       <c r="F28" t="s">
-        <v>240</v>
+        <v>304</v>
       </c>
       <c r="G28" t="s">
-        <v>243</v>
+        <v>305</v>
       </c>
       <c r="H28" t="s">
-        <v>244</v>
+        <v>306</v>
       </c>
       <c r="I28" t="s">
-        <v>245</v>
+        <v>307</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
       <c r="B29" t="s">
-        <v>246</v>
+        <v>183</v>
       </c>
       <c r="C29" t="s">
-        <v>246</v>
+        <v>183</v>
       </c>
       <c r="D29" t="s">
-        <v>247</v>
+        <v>183</v>
       </c>
       <c r="E29" t="s">
-        <v>248</v>
+        <v>184</v>
       </c>
       <c r="F29" t="s">
-        <v>246</v>
+        <v>185</v>
       </c>
       <c r="G29" t="s">
-        <v>248</v>
+        <v>183</v>
       </c>
       <c r="H29" t="s">
-        <v>249</v>
+        <v>186</v>
       </c>
       <c r="I29" t="s">
-        <v>250</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="B30" t="s">
-        <v>251</v>
+        <v>486</v>
       </c>
       <c r="C30" t="s">
-        <v>252</v>
+        <v>486</v>
       </c>
       <c r="D30" t="s">
-        <v>253</v>
+        <v>486</v>
       </c>
       <c r="E30" t="s">
-        <v>254</v>
+        <v>486</v>
       </c>
       <c r="F30" t="s">
-        <v>255</v>
+        <v>487</v>
       </c>
       <c r="G30" t="s">
-        <v>256</v>
+        <v>486</v>
       </c>
       <c r="H30" t="s">
-        <v>257</v>
+        <v>488</v>
       </c>
       <c r="I30" t="s">
-        <v>258</v>
+        <v>489</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>587</v>
+        <v>1000</v>
       </c>
       <c r="B31" t="s">
-        <v>259</v>
+        <v>1001</v>
       </c>
       <c r="C31" t="s">
-        <v>259</v>
+        <v>1001</v>
       </c>
       <c r="D31" t="s">
-        <v>259</v>
+        <v>1002</v>
       </c>
       <c r="E31" t="s">
-        <v>259</v>
+        <v>1003</v>
       </c>
       <c r="F31" t="s">
-        <v>259</v>
+        <v>1004</v>
       </c>
       <c r="G31" t="s">
-        <v>259</v>
+        <v>1005</v>
       </c>
       <c r="H31" t="s">
-        <v>260</v>
+        <v>1006</v>
       </c>
       <c r="I31" t="s">
-        <v>261</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -5545,1800 +5645,1945 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>589</v>
+        <v>573</v>
       </c>
       <c r="B33" t="s">
-        <v>265</v>
+        <v>175</v>
       </c>
       <c r="C33" t="s">
-        <v>266</v>
+        <v>176</v>
       </c>
       <c r="D33" t="s">
-        <v>267</v>
+        <v>177</v>
       </c>
       <c r="E33" t="s">
-        <v>268</v>
+        <v>178</v>
       </c>
       <c r="F33" t="s">
-        <v>269</v>
+        <v>179</v>
       </c>
       <c r="G33" t="s">
-        <v>268</v>
+        <v>180</v>
       </c>
       <c r="H33" t="s">
-        <v>270</v>
+        <v>181</v>
       </c>
       <c r="I33" t="s">
-        <v>271</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>590</v>
+        <v>998</v>
       </c>
       <c r="B34" t="s">
-        <v>272</v>
+        <v>993</v>
       </c>
       <c r="C34" t="s">
-        <v>273</v>
+        <v>994</v>
       </c>
       <c r="D34" t="s">
-        <v>274</v>
+        <v>993</v>
       </c>
       <c r="E34" t="s">
-        <v>275</v>
+        <v>993</v>
       </c>
       <c r="F34" t="s">
-        <v>276</v>
+        <v>993</v>
       </c>
       <c r="G34" t="s">
-        <v>277</v>
+        <v>995</v>
       </c>
       <c r="H34" t="s">
-        <v>278</v>
+        <v>996</v>
       </c>
       <c r="I34" t="s">
-        <v>279</v>
+        <v>997</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>731</v>
+        <v>590</v>
       </c>
       <c r="B35" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C35" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D35" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="E35" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F35" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="G35" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="H35" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="I35" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>591</v>
+        <v>568</v>
       </c>
       <c r="B36" t="s">
-        <v>286</v>
+        <v>145</v>
       </c>
       <c r="C36" t="s">
-        <v>287</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
-        <v>286</v>
+        <v>147</v>
       </c>
       <c r="E36" t="s">
-        <v>288</v>
+        <v>148</v>
       </c>
       <c r="F36" t="s">
-        <v>289</v>
+        <v>149</v>
       </c>
       <c r="G36" t="s">
-        <v>290</v>
+        <v>150</v>
       </c>
       <c r="H36" t="s">
-        <v>291</v>
+        <v>151</v>
       </c>
       <c r="I36" t="s">
-        <v>292</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>592</v>
+        <v>601</v>
       </c>
       <c r="B37" t="s">
-        <v>293</v>
+        <v>366</v>
       </c>
       <c r="C37" t="s">
-        <v>294</v>
+        <v>366</v>
       </c>
       <c r="D37" t="s">
-        <v>293</v>
+        <v>366</v>
       </c>
       <c r="E37" t="s">
-        <v>295</v>
+        <v>367</v>
       </c>
       <c r="F37" t="s">
-        <v>296</v>
+        <v>366</v>
       </c>
       <c r="G37" t="s">
-        <v>297</v>
+        <v>366</v>
       </c>
       <c r="H37" t="s">
-        <v>298</v>
+        <v>368</v>
       </c>
       <c r="I37" t="s">
-        <v>299</v>
+        <v>369</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="B38" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="C38" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="D38" t="s">
-        <v>302</v>
+        <v>267</v>
       </c>
       <c r="E38" t="s">
-        <v>303</v>
+        <v>268</v>
       </c>
       <c r="F38" t="s">
-        <v>304</v>
+        <v>269</v>
       </c>
       <c r="G38" t="s">
-        <v>305</v>
+        <v>268</v>
       </c>
       <c r="H38" t="s">
-        <v>306</v>
+        <v>270</v>
       </c>
       <c r="I38" t="s">
-        <v>307</v>
+        <v>271</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>594</v>
+        <v>562</v>
       </c>
       <c r="B39" t="s">
-        <v>308</v>
+        <v>105</v>
       </c>
       <c r="C39" t="s">
-        <v>309</v>
+        <v>106</v>
       </c>
       <c r="D39" t="s">
-        <v>308</v>
+        <v>107</v>
       </c>
       <c r="E39" t="s">
-        <v>308</v>
+        <v>108</v>
       </c>
       <c r="F39" t="s">
-        <v>310</v>
+        <v>105</v>
       </c>
       <c r="G39" t="s">
-        <v>308</v>
+        <v>109</v>
       </c>
       <c r="H39" t="s">
-        <v>311</v>
+        <v>110</v>
       </c>
       <c r="I39" t="s">
-        <v>312</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>595</v>
+        <v>564</v>
       </c>
       <c r="B40" t="s">
-        <v>313</v>
+        <v>119</v>
       </c>
       <c r="C40" t="s">
-        <v>314</v>
+        <v>120</v>
       </c>
       <c r="D40" t="s">
-        <v>315</v>
+        <v>121</v>
       </c>
       <c r="E40" t="s">
-        <v>316</v>
+        <v>122</v>
       </c>
       <c r="F40" t="s">
-        <v>317</v>
+        <v>123</v>
       </c>
       <c r="G40" t="s">
-        <v>318</v>
+        <v>124</v>
       </c>
       <c r="H40" t="s">
-        <v>319</v>
+        <v>125</v>
       </c>
       <c r="I40" t="s">
-        <v>320</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>596</v>
+        <v>612</v>
       </c>
       <c r="B41" t="s">
-        <v>321</v>
+        <v>427</v>
       </c>
       <c r="C41" t="s">
-        <v>322</v>
+        <v>428</v>
       </c>
       <c r="D41" t="s">
-        <v>323</v>
+        <v>428</v>
       </c>
       <c r="E41" t="s">
-        <v>324</v>
+        <v>429</v>
       </c>
       <c r="F41" t="s">
-        <v>325</v>
+        <v>430</v>
       </c>
       <c r="G41" t="s">
-        <v>326</v>
+        <v>427</v>
       </c>
       <c r="H41" t="s">
-        <v>327</v>
+        <v>431</v>
       </c>
       <c r="I41" t="s">
-        <v>328</v>
+        <v>432</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>597</v>
+        <v>560</v>
       </c>
       <c r="B42" t="s">
-        <v>329</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>330</v>
+        <v>95</v>
       </c>
       <c r="D42" t="s">
-        <v>331</v>
+        <v>95</v>
       </c>
       <c r="E42" t="s">
-        <v>332</v>
+        <v>94</v>
       </c>
       <c r="F42" t="s">
-        <v>333</v>
+        <v>96</v>
       </c>
       <c r="G42" t="s">
-        <v>334</v>
+        <v>97</v>
       </c>
       <c r="H42" t="s">
-        <v>335</v>
+        <v>98</v>
       </c>
       <c r="I42" t="s">
-        <v>336</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>598</v>
+        <v>732</v>
       </c>
       <c r="B43" t="s">
-        <v>337</v>
+        <v>733</v>
       </c>
       <c r="C43" t="s">
-        <v>337</v>
+        <v>733</v>
       </c>
       <c r="D43" t="s">
-        <v>337</v>
+        <v>733</v>
       </c>
       <c r="E43" t="s">
-        <v>338</v>
+        <v>734</v>
       </c>
       <c r="F43" t="s">
-        <v>339</v>
+        <v>733</v>
       </c>
       <c r="G43" t="s">
-        <v>340</v>
+        <v>735</v>
       </c>
       <c r="H43" t="s">
-        <v>341</v>
+        <v>736</v>
       </c>
       <c r="I43" t="s">
-        <v>342</v>
+        <v>737</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>599</v>
+        <v>569</v>
       </c>
       <c r="B44" t="s">
-        <v>343</v>
+        <v>153</v>
       </c>
       <c r="C44" t="s">
-        <v>344</v>
+        <v>154</v>
       </c>
       <c r="D44" t="s">
-        <v>345</v>
+        <v>155</v>
       </c>
       <c r="E44" t="s">
-        <v>346</v>
+        <v>156</v>
       </c>
       <c r="F44" t="s">
-        <v>347</v>
+        <v>157</v>
       </c>
       <c r="G44" t="s">
-        <v>348</v>
+        <v>158</v>
       </c>
       <c r="H44" t="s">
-        <v>349</v>
+        <v>159</v>
       </c>
       <c r="I44" t="s">
-        <v>350</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>600</v>
+        <v>615</v>
       </c>
       <c r="B45" t="s">
-        <v>351</v>
+        <v>444</v>
       </c>
       <c r="C45" t="s">
-        <v>352</v>
+        <v>444</v>
       </c>
       <c r="D45" t="s">
-        <v>351</v>
+        <v>444</v>
       </c>
       <c r="E45" t="s">
-        <v>353</v>
+        <v>444</v>
       </c>
       <c r="F45" t="s">
-        <v>354</v>
+        <v>444</v>
       </c>
       <c r="G45" t="s">
-        <v>355</v>
+        <v>444</v>
       </c>
       <c r="H45" t="s">
-        <v>356</v>
+        <v>445</v>
       </c>
       <c r="I45" t="s">
-        <v>357</v>
+        <v>446</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>730</v>
+        <v>610</v>
       </c>
       <c r="B46" t="s">
-        <v>358</v>
+        <v>417</v>
       </c>
       <c r="C46" t="s">
-        <v>359</v>
+        <v>418</v>
       </c>
       <c r="D46" t="s">
-        <v>360</v>
+        <v>418</v>
       </c>
       <c r="E46" t="s">
-        <v>361</v>
+        <v>419</v>
       </c>
       <c r="F46" t="s">
-        <v>362</v>
+        <v>420</v>
       </c>
       <c r="G46" t="s">
-        <v>363</v>
+        <v>421</v>
       </c>
       <c r="H46" t="s">
-        <v>364</v>
+        <v>422</v>
       </c>
       <c r="I46" t="s">
-        <v>365</v>
+        <v>423</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>601</v>
+        <v>726</v>
       </c>
       <c r="B47" t="s">
-        <v>366</v>
+        <v>715</v>
       </c>
       <c r="C47" t="s">
-        <v>366</v>
+        <v>716</v>
       </c>
       <c r="D47" t="s">
-        <v>366</v>
+        <v>715</v>
       </c>
       <c r="E47" t="s">
-        <v>367</v>
+        <v>717</v>
       </c>
       <c r="F47" t="s">
-        <v>366</v>
+        <v>715</v>
       </c>
       <c r="G47" t="s">
-        <v>366</v>
+        <v>717</v>
       </c>
       <c r="H47" t="s">
-        <v>368</v>
+        <v>718</v>
       </c>
       <c r="I47" t="s">
-        <v>369</v>
+        <v>719</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>602</v>
+        <v>628</v>
       </c>
       <c r="B48" t="s">
-        <v>370</v>
+        <v>536</v>
       </c>
       <c r="C48" t="s">
-        <v>371</v>
+        <v>536</v>
       </c>
       <c r="D48" t="s">
-        <v>371</v>
+        <v>536</v>
       </c>
       <c r="E48" t="s">
-        <v>372</v>
+        <v>536</v>
       </c>
       <c r="F48" t="s">
-        <v>373</v>
+        <v>536</v>
       </c>
       <c r="G48" t="s">
-        <v>374</v>
+        <v>536</v>
       </c>
       <c r="H48" t="s">
-        <v>375</v>
+        <v>537</v>
       </c>
       <c r="I48" t="s">
-        <v>376</v>
+        <v>538</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="B49" t="s">
-        <v>377</v>
+        <v>321</v>
       </c>
       <c r="C49" t="s">
-        <v>378</v>
+        <v>322</v>
       </c>
       <c r="D49" t="s">
-        <v>377</v>
+        <v>323</v>
       </c>
       <c r="E49" t="s">
-        <v>379</v>
+        <v>324</v>
       </c>
       <c r="F49" t="s">
-        <v>380</v>
+        <v>325</v>
       </c>
       <c r="G49" t="s">
-        <v>381</v>
+        <v>326</v>
       </c>
       <c r="H49" t="s">
-        <v>382</v>
+        <v>327</v>
       </c>
       <c r="I49" t="s">
-        <v>383</v>
+        <v>328</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B50" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="C50" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="D50" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="E50" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
       <c r="F50" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="G50" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="H50" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="I50" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>605</v>
+        <v>578</v>
       </c>
       <c r="B51" t="s">
-        <v>391</v>
+        <v>206</v>
       </c>
       <c r="C51" t="s">
-        <v>391</v>
+        <v>206</v>
       </c>
       <c r="D51" t="s">
-        <v>391</v>
+        <v>206</v>
       </c>
       <c r="E51" t="s">
-        <v>391</v>
+        <v>207</v>
       </c>
       <c r="F51" t="s">
-        <v>391</v>
+        <v>206</v>
       </c>
       <c r="G51" t="s">
-        <v>391</v>
+        <v>206</v>
       </c>
       <c r="H51" t="s">
-        <v>392</v>
+        <v>208</v>
       </c>
       <c r="I51" t="s">
-        <v>393</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>606</v>
+        <v>624</v>
       </c>
       <c r="B52" t="s">
-        <v>394</v>
+        <v>510</v>
       </c>
       <c r="C52" t="s">
-        <v>394</v>
+        <v>510</v>
       </c>
       <c r="D52" t="s">
-        <v>394</v>
+        <v>510</v>
       </c>
       <c r="E52" t="s">
-        <v>394</v>
+        <v>511</v>
       </c>
       <c r="F52" t="s">
-        <v>395</v>
+        <v>511</v>
       </c>
       <c r="G52" t="s">
-        <v>394</v>
+        <v>511</v>
       </c>
       <c r="H52" t="s">
-        <v>396</v>
+        <v>512</v>
       </c>
       <c r="I52" t="s">
-        <v>397</v>
+        <v>513</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>607</v>
+        <v>618</v>
       </c>
       <c r="B53" t="s">
-        <v>398</v>
+        <v>459</v>
       </c>
       <c r="C53" t="s">
-        <v>398</v>
+        <v>460</v>
       </c>
       <c r="D53" t="s">
-        <v>398</v>
+        <v>461</v>
       </c>
       <c r="E53" t="s">
-        <v>398</v>
+        <v>462</v>
       </c>
       <c r="F53" t="s">
-        <v>398</v>
+        <v>463</v>
       </c>
       <c r="G53" t="s">
-        <v>398</v>
+        <v>464</v>
       </c>
       <c r="H53" t="s">
-        <v>399</v>
+        <v>465</v>
       </c>
       <c r="I53" t="s">
-        <v>400</v>
+        <v>466</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>608</v>
+        <v>626</v>
       </c>
       <c r="B54" t="s">
-        <v>401</v>
+        <v>520</v>
       </c>
       <c r="C54" t="s">
-        <v>402</v>
+        <v>520</v>
       </c>
       <c r="D54" t="s">
-        <v>403</v>
+        <v>521</v>
       </c>
       <c r="E54" t="s">
-        <v>404</v>
+        <v>522</v>
       </c>
       <c r="F54" t="s">
-        <v>405</v>
+        <v>520</v>
       </c>
       <c r="G54" t="s">
-        <v>406</v>
+        <v>522</v>
       </c>
       <c r="H54" t="s">
-        <v>407</v>
+        <v>523</v>
       </c>
       <c r="I54" t="s">
-        <v>408</v>
+        <v>524</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>609</v>
+        <v>563</v>
       </c>
       <c r="B55" t="s">
-        <v>409</v>
+        <v>112</v>
       </c>
       <c r="C55" t="s">
-        <v>410</v>
+        <v>113</v>
       </c>
       <c r="D55" t="s">
-        <v>411</v>
+        <v>113</v>
       </c>
       <c r="E55" t="s">
-        <v>412</v>
+        <v>114</v>
       </c>
       <c r="F55" t="s">
-        <v>413</v>
+        <v>115</v>
       </c>
       <c r="G55" t="s">
-        <v>414</v>
+        <v>116</v>
       </c>
       <c r="H55" t="s">
-        <v>415</v>
+        <v>117</v>
       </c>
       <c r="I55" t="s">
-        <v>416</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B56" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
       <c r="C56" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="D56" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="E56" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="F56" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
       <c r="G56" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="H56" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="I56" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>611</v>
+        <v>756</v>
       </c>
       <c r="B57" t="s">
-        <v>424</v>
+        <v>467</v>
       </c>
       <c r="C57" t="s">
-        <v>424</v>
+        <v>467</v>
       </c>
       <c r="D57" t="s">
-        <v>424</v>
+        <v>468</v>
       </c>
       <c r="E57" t="s">
-        <v>424</v>
+        <v>469</v>
       </c>
       <c r="F57" t="s">
-        <v>424</v>
+        <v>470</v>
       </c>
       <c r="G57" t="s">
-        <v>424</v>
+        <v>467</v>
       </c>
       <c r="H57" t="s">
-        <v>425</v>
+        <v>471</v>
       </c>
       <c r="I57" t="s">
-        <v>426</v>
+        <v>472</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>612</v>
+        <v>1008</v>
       </c>
       <c r="B58" t="s">
-        <v>427</v>
+        <v>1009</v>
       </c>
       <c r="C58" t="s">
-        <v>428</v>
+        <v>1010</v>
       </c>
       <c r="D58" t="s">
-        <v>428</v>
+        <v>1011</v>
       </c>
       <c r="E58" t="s">
-        <v>429</v>
+        <v>1012</v>
       </c>
       <c r="F58" t="s">
-        <v>430</v>
+        <v>1013</v>
       </c>
       <c r="G58" t="s">
-        <v>427</v>
+        <v>1014</v>
       </c>
       <c r="H58" t="s">
-        <v>431</v>
+        <v>1015</v>
       </c>
       <c r="I58" t="s">
-        <v>432</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>613</v>
+        <v>580</v>
       </c>
       <c r="B59" t="s">
-        <v>433</v>
+        <v>216</v>
       </c>
       <c r="C59" t="s">
-        <v>433</v>
+        <v>217</v>
       </c>
       <c r="D59" t="s">
-        <v>433</v>
+        <v>218</v>
       </c>
       <c r="E59" t="s">
-        <v>433</v>
+        <v>219</v>
       </c>
       <c r="F59" t="s">
-        <v>433</v>
+        <v>216</v>
       </c>
       <c r="G59" t="s">
-        <v>433</v>
+        <v>216</v>
       </c>
       <c r="H59" t="s">
-        <v>434</v>
+        <v>220</v>
       </c>
       <c r="I59" t="s">
-        <v>435</v>
+        <v>221</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>614</v>
+        <v>586</v>
       </c>
       <c r="B60" t="s">
-        <v>436</v>
+        <v>251</v>
       </c>
       <c r="C60" t="s">
-        <v>437</v>
+        <v>252</v>
       </c>
       <c r="D60" t="s">
-        <v>438</v>
+        <v>253</v>
       </c>
       <c r="E60" t="s">
-        <v>439</v>
+        <v>254</v>
       </c>
       <c r="F60" t="s">
-        <v>440</v>
+        <v>255</v>
       </c>
       <c r="G60" t="s">
-        <v>441</v>
+        <v>256</v>
       </c>
       <c r="H60" t="s">
-        <v>442</v>
+        <v>257</v>
       </c>
       <c r="I60" t="s">
-        <v>443</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="B61" t="s">
-        <v>444</v>
+        <v>384</v>
       </c>
       <c r="C61" t="s">
-        <v>444</v>
+        <v>385</v>
       </c>
       <c r="D61" t="s">
-        <v>444</v>
+        <v>385</v>
       </c>
       <c r="E61" t="s">
-        <v>444</v>
+        <v>386</v>
       </c>
       <c r="F61" t="s">
-        <v>444</v>
+        <v>387</v>
       </c>
       <c r="G61" t="s">
-        <v>444</v>
+        <v>388</v>
       </c>
       <c r="H61" t="s">
-        <v>445</v>
+        <v>389</v>
       </c>
       <c r="I61" t="s">
-        <v>446</v>
+        <v>390</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
       <c r="B62" t="s">
-        <v>447</v>
+        <v>398</v>
       </c>
       <c r="C62" t="s">
-        <v>448</v>
+        <v>398</v>
       </c>
       <c r="D62" t="s">
-        <v>447</v>
+        <v>398</v>
       </c>
       <c r="E62" t="s">
-        <v>447</v>
+        <v>398</v>
       </c>
       <c r="F62" t="s">
-        <v>447</v>
+        <v>398</v>
       </c>
       <c r="G62" t="s">
-        <v>447</v>
+        <v>398</v>
       </c>
       <c r="H62" t="s">
-        <v>449</v>
+        <v>399</v>
       </c>
       <c r="I62" t="s">
-        <v>450</v>
+        <v>400</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>617</v>
+        <v>581</v>
       </c>
       <c r="B63" t="s">
-        <v>451</v>
+        <v>222</v>
       </c>
       <c r="C63" t="s">
-        <v>452</v>
+        <v>223</v>
       </c>
       <c r="D63" t="s">
-        <v>453</v>
+        <v>224</v>
       </c>
       <c r="E63" t="s">
-        <v>454</v>
+        <v>225</v>
       </c>
       <c r="F63" t="s">
-        <v>455</v>
+        <v>226</v>
       </c>
       <c r="G63" t="s">
-        <v>456</v>
+        <v>226</v>
       </c>
       <c r="H63" t="s">
-        <v>457</v>
+        <v>227</v>
       </c>
       <c r="I63" t="s">
-        <v>458</v>
+        <v>693</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>618</v>
+        <v>566</v>
       </c>
       <c r="B64" t="s">
-        <v>459</v>
+        <v>130</v>
       </c>
       <c r="C64" t="s">
-        <v>460</v>
+        <v>131</v>
       </c>
       <c r="D64" t="s">
-        <v>461</v>
+        <v>132</v>
       </c>
       <c r="E64" t="s">
-        <v>462</v>
+        <v>133</v>
       </c>
       <c r="F64" t="s">
-        <v>463</v>
+        <v>134</v>
       </c>
       <c r="G64" t="s">
-        <v>464</v>
+        <v>130</v>
       </c>
       <c r="H64" t="s">
-        <v>465</v>
+        <v>135</v>
       </c>
       <c r="I64" t="s">
-        <v>466</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>756</v>
+        <v>623</v>
       </c>
       <c r="B65" t="s">
-        <v>467</v>
+        <v>506</v>
       </c>
       <c r="C65" t="s">
-        <v>467</v>
+        <v>506</v>
       </c>
       <c r="D65" t="s">
-        <v>468</v>
+        <v>506</v>
       </c>
       <c r="E65" t="s">
-        <v>469</v>
+        <v>507</v>
       </c>
       <c r="F65" t="s">
-        <v>470</v>
+        <v>506</v>
       </c>
       <c r="G65" t="s">
-        <v>467</v>
+        <v>506</v>
       </c>
       <c r="H65" t="s">
-        <v>471</v>
+        <v>508</v>
       </c>
       <c r="I65" t="s">
-        <v>472</v>
+        <v>509</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>729</v>
+        <v>567</v>
       </c>
       <c r="B66" t="s">
-        <v>473</v>
+        <v>137</v>
       </c>
       <c r="C66" t="s">
-        <v>474</v>
+        <v>138</v>
       </c>
       <c r="D66" t="s">
-        <v>473</v>
+        <v>139</v>
       </c>
       <c r="E66" t="s">
-        <v>475</v>
+        <v>140</v>
       </c>
       <c r="F66" t="s">
-        <v>476</v>
+        <v>141</v>
       </c>
       <c r="G66" t="s">
-        <v>477</v>
+        <v>142</v>
       </c>
       <c r="H66" t="s">
-        <v>478</v>
+        <v>143</v>
       </c>
       <c r="I66" t="s">
-        <v>479</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>619</v>
+        <v>587</v>
       </c>
       <c r="B67" t="s">
-        <v>480</v>
+        <v>259</v>
       </c>
       <c r="C67" t="s">
-        <v>480</v>
+        <v>259</v>
       </c>
       <c r="D67" t="s">
-        <v>480</v>
+        <v>259</v>
       </c>
       <c r="E67" t="s">
-        <v>481</v>
+        <v>259</v>
       </c>
       <c r="F67" t="s">
-        <v>482</v>
+        <v>259</v>
       </c>
       <c r="G67" t="s">
-        <v>483</v>
+        <v>259</v>
       </c>
       <c r="H67" t="s">
-        <v>484</v>
+        <v>260</v>
       </c>
       <c r="I67" t="s">
-        <v>485</v>
+        <v>261</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="B68" t="s">
-        <v>486</v>
+        <v>409</v>
       </c>
       <c r="C68" t="s">
-        <v>486</v>
+        <v>410</v>
       </c>
       <c r="D68" t="s">
-        <v>486</v>
+        <v>411</v>
       </c>
       <c r="E68" t="s">
-        <v>486</v>
+        <v>412</v>
       </c>
       <c r="F68" t="s">
-        <v>487</v>
+        <v>413</v>
       </c>
       <c r="G68" t="s">
-        <v>486</v>
+        <v>414</v>
       </c>
       <c r="H68" t="s">
-        <v>488</v>
+        <v>415</v>
       </c>
       <c r="I68" t="s">
-        <v>489</v>
+        <v>416</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="B69" t="s">
-        <v>490</v>
+        <v>451</v>
       </c>
       <c r="C69" t="s">
-        <v>491</v>
+        <v>452</v>
       </c>
       <c r="D69" t="s">
-        <v>492</v>
+        <v>453</v>
       </c>
       <c r="E69" t="s">
-        <v>493</v>
+        <v>454</v>
       </c>
       <c r="F69" t="s">
-        <v>494</v>
+        <v>455</v>
       </c>
       <c r="G69" t="s">
-        <v>495</v>
+        <v>456</v>
       </c>
       <c r="H69" t="s">
-        <v>496</v>
+        <v>457</v>
       </c>
       <c r="I69" t="s">
-        <v>497</v>
+        <v>458</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>622</v>
+        <v>597</v>
       </c>
       <c r="B70" t="s">
-        <v>498</v>
+        <v>329</v>
       </c>
       <c r="C70" t="s">
-        <v>499</v>
+        <v>330</v>
       </c>
       <c r="D70" t="s">
-        <v>500</v>
+        <v>331</v>
       </c>
       <c r="E70" t="s">
-        <v>501</v>
+        <v>332</v>
       </c>
       <c r="F70" t="s">
-        <v>502</v>
+        <v>333</v>
       </c>
       <c r="G70" t="s">
-        <v>503</v>
+        <v>334</v>
       </c>
       <c r="H70" t="s">
-        <v>504</v>
+        <v>335</v>
       </c>
       <c r="I70" t="s">
-        <v>505</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>623</v>
+        <v>723</v>
       </c>
       <c r="B71" t="s">
-        <v>506</v>
+        <v>695</v>
       </c>
       <c r="C71" t="s">
-        <v>506</v>
+        <v>696</v>
       </c>
       <c r="D71" t="s">
-        <v>506</v>
+        <v>697</v>
       </c>
       <c r="E71" t="s">
-        <v>507</v>
+        <v>698</v>
       </c>
       <c r="F71" t="s">
-        <v>506</v>
+        <v>699</v>
       </c>
       <c r="G71" t="s">
-        <v>506</v>
+        <v>700</v>
       </c>
       <c r="H71" t="s">
-        <v>508</v>
+        <v>701</v>
       </c>
       <c r="I71" t="s">
-        <v>509</v>
+        <v>702</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="B72" t="s">
-        <v>510</v>
+        <v>447</v>
       </c>
       <c r="C72" t="s">
-        <v>510</v>
+        <v>448</v>
       </c>
       <c r="D72" t="s">
-        <v>510</v>
+        <v>447</v>
       </c>
       <c r="E72" t="s">
-        <v>511</v>
+        <v>447</v>
       </c>
       <c r="F72" t="s">
-        <v>511</v>
+        <v>447</v>
       </c>
       <c r="G72" t="s">
-        <v>511</v>
+        <v>447</v>
       </c>
       <c r="H72" t="s">
-        <v>512</v>
+        <v>449</v>
       </c>
       <c r="I72" t="s">
-        <v>513</v>
+        <v>450</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>625</v>
+        <v>605</v>
       </c>
       <c r="B73" t="s">
-        <v>514</v>
+        <v>391</v>
       </c>
       <c r="C73" t="s">
-        <v>514</v>
+        <v>391</v>
       </c>
       <c r="D73" t="s">
-        <v>514</v>
+        <v>391</v>
       </c>
       <c r="E73" t="s">
-        <v>515</v>
+        <v>391</v>
       </c>
       <c r="F73" t="s">
-        <v>516</v>
+        <v>391</v>
       </c>
       <c r="G73" t="s">
-        <v>517</v>
+        <v>391</v>
       </c>
       <c r="H73" t="s">
-        <v>518</v>
+        <v>392</v>
       </c>
       <c r="I73" t="s">
-        <v>519</v>
+        <v>393</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>626</v>
+        <v>579</v>
       </c>
       <c r="B74" t="s">
-        <v>520</v>
+        <v>210</v>
       </c>
       <c r="C74" t="s">
-        <v>520</v>
+        <v>211</v>
       </c>
       <c r="D74" t="s">
-        <v>521</v>
+        <v>212</v>
       </c>
       <c r="E74" t="s">
-        <v>522</v>
+        <v>213</v>
       </c>
       <c r="F74" t="s">
-        <v>520</v>
+        <v>210</v>
       </c>
       <c r="G74" t="s">
-        <v>522</v>
+        <v>210</v>
       </c>
       <c r="H74" t="s">
-        <v>523</v>
+        <v>214</v>
       </c>
       <c r="I74" t="s">
-        <v>524</v>
+        <v>215</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>585</v>
+        <v>724</v>
       </c>
       <c r="B75" t="s">
-        <v>525</v>
+        <v>703</v>
       </c>
       <c r="C75" t="s">
-        <v>525</v>
+        <v>704</v>
       </c>
       <c r="D75" t="s">
-        <v>526</v>
+        <v>705</v>
       </c>
       <c r="E75" t="s">
-        <v>527</v>
+        <v>703</v>
       </c>
       <c r="F75" t="s">
-        <v>525</v>
+        <v>706</v>
       </c>
       <c r="G75" t="s">
-        <v>525</v>
+        <v>707</v>
       </c>
       <c r="H75" t="s">
-        <v>528</v>
+        <v>708</v>
       </c>
       <c r="I75" t="s">
-        <v>529</v>
+        <v>709</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>627</v>
+        <v>583</v>
       </c>
       <c r="B76" t="s">
-        <v>530</v>
+        <v>234</v>
       </c>
       <c r="C76" t="s">
-        <v>530</v>
+        <v>235</v>
       </c>
       <c r="D76" t="s">
-        <v>530</v>
+        <v>235</v>
       </c>
       <c r="E76" t="s">
-        <v>531</v>
+        <v>236</v>
       </c>
       <c r="F76" t="s">
-        <v>532</v>
+        <v>237</v>
       </c>
       <c r="G76" t="s">
-        <v>533</v>
+        <v>237</v>
       </c>
       <c r="H76" t="s">
-        <v>534</v>
+        <v>238</v>
       </c>
       <c r="I76" t="s">
-        <v>535</v>
+        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>628</v>
+        <v>565</v>
       </c>
       <c r="B77" t="s">
-        <v>536</v>
+        <v>127</v>
       </c>
       <c r="C77" t="s">
-        <v>536</v>
+        <v>127</v>
       </c>
       <c r="D77" t="s">
-        <v>536</v>
+        <v>128</v>
       </c>
       <c r="E77" t="s">
-        <v>536</v>
+        <v>127</v>
       </c>
       <c r="F77" t="s">
-        <v>536</v>
+        <v>127</v>
       </c>
       <c r="G77" t="s">
-        <v>536</v>
+        <v>127</v>
       </c>
       <c r="H77" t="s">
-        <v>537</v>
+        <v>129</v>
       </c>
       <c r="I77" t="s">
-        <v>538</v>
+        <v>690</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="B78" t="s">
-        <v>539</v>
+        <v>394</v>
       </c>
       <c r="C78" t="s">
-        <v>540</v>
+        <v>394</v>
       </c>
       <c r="D78" t="s">
-        <v>539</v>
+        <v>394</v>
       </c>
       <c r="E78" t="s">
-        <v>541</v>
+        <v>394</v>
       </c>
       <c r="F78" t="s">
-        <v>539</v>
+        <v>395</v>
       </c>
       <c r="G78" t="s">
-        <v>540</v>
+        <v>394</v>
       </c>
       <c r="H78" t="s">
-        <v>542</v>
+        <v>396</v>
       </c>
       <c r="I78" t="s">
-        <v>543</v>
+        <v>397</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>629</v>
+        <v>603</v>
       </c>
       <c r="B79" t="s">
-        <v>544</v>
+        <v>377</v>
       </c>
       <c r="C79" t="s">
-        <v>544</v>
+        <v>378</v>
       </c>
       <c r="D79" t="s">
-        <v>544</v>
+        <v>377</v>
       </c>
       <c r="E79" t="s">
-        <v>545</v>
+        <v>379</v>
       </c>
       <c r="F79" t="s">
-        <v>546</v>
+        <v>380</v>
       </c>
       <c r="G79" t="s">
-        <v>547</v>
+        <v>381</v>
       </c>
       <c r="H79" t="s">
-        <v>548</v>
+        <v>382</v>
       </c>
       <c r="I79" t="s">
-        <v>549</v>
+        <v>383</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>630</v>
+        <v>592</v>
       </c>
       <c r="B80" t="s">
-        <v>550</v>
+        <v>293</v>
       </c>
       <c r="C80" t="s">
-        <v>551</v>
+        <v>294</v>
       </c>
       <c r="D80" t="s">
-        <v>552</v>
+        <v>293</v>
       </c>
       <c r="E80" t="s">
-        <v>553</v>
+        <v>295</v>
       </c>
       <c r="F80" t="s">
-        <v>554</v>
+        <v>296</v>
       </c>
       <c r="G80" t="s">
-        <v>555</v>
+        <v>297</v>
       </c>
       <c r="H80" t="s">
-        <v>556</v>
+        <v>298</v>
       </c>
       <c r="I80" t="s">
-        <v>557</v>
+        <v>299</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>723</v>
+        <v>622</v>
       </c>
       <c r="B81" t="s">
-        <v>695</v>
+        <v>498</v>
       </c>
       <c r="C81" t="s">
-        <v>696</v>
+        <v>499</v>
       </c>
       <c r="D81" t="s">
-        <v>697</v>
+        <v>500</v>
       </c>
       <c r="E81" t="s">
-        <v>698</v>
+        <v>501</v>
       </c>
       <c r="F81" t="s">
-        <v>699</v>
+        <v>502</v>
       </c>
       <c r="G81" t="s">
-        <v>700</v>
+        <v>503</v>
       </c>
       <c r="H81" t="s">
-        <v>701</v>
+        <v>504</v>
       </c>
       <c r="I81" t="s">
-        <v>702</v>
+        <v>505</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>724</v>
+        <v>595</v>
       </c>
       <c r="B82" t="s">
-        <v>703</v>
+        <v>313</v>
       </c>
       <c r="C82" t="s">
-        <v>704</v>
+        <v>314</v>
       </c>
       <c r="D82" t="s">
-        <v>705</v>
+        <v>315</v>
       </c>
       <c r="E82" t="s">
-        <v>703</v>
+        <v>316</v>
       </c>
       <c r="F82" t="s">
-        <v>706</v>
+        <v>317</v>
       </c>
       <c r="G82" t="s">
-        <v>707</v>
+        <v>318</v>
       </c>
       <c r="H82" t="s">
-        <v>708</v>
+        <v>319</v>
       </c>
       <c r="I82" t="s">
-        <v>709</v>
+        <v>320</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>725</v>
+        <v>577</v>
       </c>
       <c r="B83" t="s">
-        <v>710</v>
+        <v>202</v>
       </c>
       <c r="C83" t="s">
-        <v>710</v>
+        <v>202</v>
       </c>
       <c r="D83" t="s">
-        <v>710</v>
+        <v>202</v>
       </c>
       <c r="E83" t="s">
-        <v>711</v>
+        <v>203</v>
       </c>
       <c r="F83" t="s">
-        <v>712</v>
+        <v>202</v>
       </c>
       <c r="G83" t="s">
-        <v>710</v>
+        <v>202</v>
       </c>
       <c r="H83" t="s">
-        <v>713</v>
+        <v>204</v>
       </c>
       <c r="I83" t="s">
-        <v>714</v>
+        <v>205</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>726</v>
+        <v>582</v>
       </c>
       <c r="B84" t="s">
-        <v>715</v>
+        <v>228</v>
       </c>
       <c r="C84" t="s">
-        <v>716</v>
+        <v>228</v>
       </c>
       <c r="D84" t="s">
-        <v>715</v>
+        <v>228</v>
       </c>
       <c r="E84" t="s">
-        <v>717</v>
+        <v>229</v>
       </c>
       <c r="F84" t="s">
-        <v>715</v>
+        <v>230</v>
       </c>
       <c r="G84" t="s">
-        <v>717</v>
+        <v>231</v>
       </c>
       <c r="H84" t="s">
-        <v>718</v>
+        <v>232</v>
       </c>
       <c r="I84" t="s">
-        <v>719</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>727</v>
+        <v>571</v>
       </c>
       <c r="B85" t="s">
-        <v>720</v>
+        <v>163</v>
       </c>
       <c r="C85" t="s">
-        <v>720</v>
+        <v>164</v>
       </c>
       <c r="D85" t="s">
-        <v>720</v>
+        <v>165</v>
       </c>
       <c r="E85" t="s">
-        <v>720</v>
+        <v>166</v>
       </c>
       <c r="F85" t="s">
-        <v>720</v>
+        <v>167</v>
       </c>
       <c r="G85" t="s">
-        <v>720</v>
+        <v>168</v>
       </c>
       <c r="H85" t="s">
-        <v>721</v>
+        <v>169</v>
       </c>
       <c r="I85" t="s">
-        <v>722</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B86" t="s">
-        <v>733</v>
+        <v>358</v>
       </c>
       <c r="C86" t="s">
-        <v>733</v>
+        <v>359</v>
       </c>
       <c r="D86" t="s">
-        <v>733</v>
+        <v>360</v>
       </c>
       <c r="E86" t="s">
-        <v>734</v>
+        <v>361</v>
       </c>
       <c r="F86" t="s">
-        <v>733</v>
+        <v>362</v>
       </c>
       <c r="G86" t="s">
-        <v>735</v>
+        <v>363</v>
       </c>
       <c r="H86" t="s">
-        <v>736</v>
+        <v>364</v>
       </c>
       <c r="I86" t="s">
-        <v>737</v>
+        <v>365</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>985</v>
+        <v>729</v>
       </c>
       <c r="B87" t="s">
-        <v>945</v>
+        <v>473</v>
       </c>
       <c r="C87" t="s">
-        <v>946</v>
+        <v>474</v>
       </c>
       <c r="D87" t="s">
-        <v>945</v>
+        <v>473</v>
       </c>
       <c r="E87" t="s">
-        <v>947</v>
+        <v>475</v>
       </c>
       <c r="F87" t="s">
-        <v>945</v>
+        <v>476</v>
       </c>
       <c r="G87" t="s">
-        <v>945</v>
+        <v>477</v>
       </c>
       <c r="H87" t="s">
-        <v>948</v>
+        <v>478</v>
       </c>
       <c r="I87" t="s">
-        <v>949</v>
+        <v>479</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>986</v>
+        <v>576</v>
       </c>
       <c r="B88" t="s">
-        <v>950</v>
+        <v>194</v>
       </c>
       <c r="C88" t="s">
-        <v>951</v>
+        <v>195</v>
       </c>
       <c r="D88" t="s">
-        <v>950</v>
+        <v>196</v>
       </c>
       <c r="E88" t="s">
-        <v>952</v>
+        <v>197</v>
       </c>
       <c r="F88" t="s">
-        <v>950</v>
+        <v>198</v>
       </c>
       <c r="G88" t="s">
-        <v>950</v>
+        <v>199</v>
       </c>
       <c r="H88" t="s">
-        <v>953</v>
+        <v>200</v>
       </c>
       <c r="I88" t="s">
-        <v>954</v>
+        <v>201</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>987</v>
+        <v>591</v>
       </c>
       <c r="B89" t="s">
-        <v>955</v>
+        <v>286</v>
       </c>
       <c r="C89" t="s">
-        <v>956</v>
+        <v>287</v>
       </c>
       <c r="D89" t="s">
-        <v>955</v>
+        <v>286</v>
       </c>
       <c r="E89" t="s">
-        <v>957</v>
+        <v>288</v>
       </c>
       <c r="F89" t="s">
-        <v>955</v>
+        <v>289</v>
       </c>
       <c r="G89" t="s">
-        <v>955</v>
+        <v>290</v>
       </c>
       <c r="H89" t="s">
-        <v>958</v>
+        <v>291</v>
       </c>
       <c r="I89" t="s">
-        <v>959</v>
+        <v>292</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>988</v>
+        <v>599</v>
       </c>
       <c r="B90" t="s">
-        <v>960</v>
+        <v>343</v>
       </c>
       <c r="C90" t="s">
-        <v>961</v>
+        <v>344</v>
       </c>
       <c r="D90" t="s">
-        <v>960</v>
+        <v>345</v>
       </c>
       <c r="E90" t="s">
-        <v>962</v>
+        <v>346</v>
       </c>
       <c r="F90" t="s">
-        <v>960</v>
+        <v>347</v>
       </c>
       <c r="G90" t="s">
-        <v>960</v>
+        <v>348</v>
       </c>
       <c r="H90" t="s">
-        <v>963</v>
+        <v>349</v>
       </c>
       <c r="I90" t="s">
-        <v>964</v>
+        <v>350</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>989</v>
+        <v>621</v>
       </c>
       <c r="B91" t="s">
-        <v>965</v>
+        <v>490</v>
       </c>
       <c r="C91" t="s">
-        <v>966</v>
+        <v>491</v>
       </c>
       <c r="D91" t="s">
-        <v>965</v>
+        <v>492</v>
       </c>
       <c r="E91" t="s">
-        <v>967</v>
+        <v>493</v>
       </c>
       <c r="F91" t="s">
-        <v>965</v>
+        <v>494</v>
       </c>
       <c r="G91" t="s">
-        <v>965</v>
+        <v>495</v>
       </c>
       <c r="H91" t="s">
-        <v>968</v>
+        <v>496</v>
       </c>
       <c r="I91" t="s">
-        <v>969</v>
+        <v>497</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>990</v>
+        <v>584</v>
       </c>
       <c r="B92" t="s">
-        <v>970</v>
+        <v>240</v>
       </c>
       <c r="C92" t="s">
-        <v>971</v>
+        <v>241</v>
       </c>
       <c r="D92" t="s">
-        <v>970</v>
+        <v>242</v>
       </c>
       <c r="E92" t="s">
-        <v>972</v>
+        <v>240</v>
       </c>
       <c r="F92" t="s">
-        <v>970</v>
+        <v>240</v>
       </c>
       <c r="G92" t="s">
-        <v>970</v>
+        <v>243</v>
       </c>
       <c r="H92" t="s">
-        <v>973</v>
+        <v>244</v>
       </c>
       <c r="I92" t="s">
-        <v>974</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>991</v>
+        <v>570</v>
       </c>
       <c r="B93" t="s">
-        <v>975</v>
+        <v>161</v>
       </c>
       <c r="C93" t="s">
-        <v>976</v>
+        <v>161</v>
       </c>
       <c r="D93" t="s">
-        <v>975</v>
+        <v>161</v>
       </c>
       <c r="E93" t="s">
-        <v>977</v>
+        <v>161</v>
       </c>
       <c r="F93" t="s">
-        <v>975</v>
+        <v>161</v>
       </c>
       <c r="G93" t="s">
-        <v>975</v>
+        <v>161</v>
       </c>
       <c r="H93" t="s">
-        <v>978</v>
+        <v>162</v>
       </c>
       <c r="I93" t="s">
-        <v>979</v>
+        <v>691</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>992</v>
+        <v>572</v>
       </c>
       <c r="B94" t="s">
-        <v>980</v>
+        <v>171</v>
       </c>
       <c r="C94" t="s">
-        <v>981</v>
+        <v>172</v>
       </c>
       <c r="D94" t="s">
-        <v>980</v>
+        <v>171</v>
       </c>
       <c r="E94" t="s">
-        <v>982</v>
+        <v>171</v>
       </c>
       <c r="F94" t="s">
-        <v>980</v>
+        <v>171</v>
       </c>
       <c r="G94" t="s">
-        <v>980</v>
+        <v>171</v>
       </c>
       <c r="H94" t="s">
-        <v>983</v>
+        <v>173</v>
       </c>
       <c r="I94" t="s">
-        <v>984</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D95" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E95" t="s">
+        <v>1020</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G95" t="s">
+        <v>1022</v>
+      </c>
+      <c r="H95" t="s">
+        <v>1023</v>
+      </c>
+      <c r="I95" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>613</v>
+      </c>
+      <c r="B96" t="s">
+        <v>433</v>
+      </c>
+      <c r="C96" t="s">
+        <v>433</v>
+      </c>
+      <c r="D96" t="s">
+        <v>433</v>
+      </c>
+      <c r="E96" t="s">
+        <v>433</v>
+      </c>
+      <c r="F96" t="s">
+        <v>433</v>
+      </c>
+      <c r="G96" t="s">
+        <v>433</v>
+      </c>
+      <c r="H96" t="s">
+        <v>434</v>
+      </c>
+      <c r="I96" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>727</v>
+      </c>
+      <c r="B97" t="s">
+        <v>720</v>
+      </c>
+      <c r="C97" t="s">
+        <v>720</v>
+      </c>
+      <c r="D97" t="s">
+        <v>720</v>
+      </c>
+      <c r="E97" t="s">
+        <v>720</v>
+      </c>
+      <c r="F97" t="s">
+        <v>720</v>
+      </c>
+      <c r="G97" t="s">
+        <v>720</v>
+      </c>
+      <c r="H97" t="s">
+        <v>721</v>
+      </c>
+      <c r="I97" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>575</v>
+      </c>
+      <c r="B98" t="s">
+        <v>188</v>
+      </c>
+      <c r="C98" t="s">
+        <v>189</v>
+      </c>
+      <c r="D98" t="s">
+        <v>190</v>
+      </c>
+      <c r="E98" t="s">
+        <v>191</v>
+      </c>
+      <c r="F98" t="s">
+        <v>188</v>
+      </c>
+      <c r="G98" t="s">
+        <v>188</v>
+      </c>
+      <c r="H98" t="s">
+        <v>192</v>
+      </c>
+      <c r="I98" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>725</v>
+      </c>
+      <c r="B99" t="s">
+        <v>710</v>
+      </c>
+      <c r="C99" t="s">
+        <v>710</v>
+      </c>
+      <c r="D99" t="s">
+        <v>710</v>
+      </c>
+      <c r="E99" t="s">
+        <v>711</v>
+      </c>
+      <c r="F99" t="s">
+        <v>712</v>
+      </c>
+      <c r="G99" t="s">
+        <v>710</v>
+      </c>
+      <c r="H99" t="s">
+        <v>713</v>
+      </c>
+      <c r="I99" t="s">
+        <v>714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shorter elimination group labels
</commit_message>
<xml_diff>
--- a/fonts/localization.xlsx
+++ b/fonts/localization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/fonts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8598DB-751A-014B-9C1F-A2788650DE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2891FBC-B2F3-EC45-9700-986EA0739A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="700" windowWidth="10020" windowHeight="19740" activeTab="5" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19740" xr2:uid="{0FA07794-2DE1-4C86-96C2-0907800AE218}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonts" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="1025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="1027">
   <si>
     <t>key</t>
   </si>
@@ -3128,6 +3128,12 @@
   </si>
   <si>
     <t>ازبکستان</t>
+  </si>
+  <si>
+    <t>match.form.label-inverse</t>
+  </si>
+  <si>
+    <t>consolai.ttf</t>
   </si>
 </sst>
 </file>
@@ -3269,8 +3275,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}" name="Table1" displayName="Table1" ref="A1:J21" totalsRowShown="0">
-  <autoFilter ref="A1:J21" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}" name="Table1" displayName="Table1" ref="A1:J22" totalsRowShown="0">
+  <autoFilter ref="A1:J22" xr:uid="{3CF181BA-F3A5-4585-9FD3-16906D63F76D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J22">
+    <sortCondition ref="A1:A22"/>
+  </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4614A9ED-E890-4F3B-BD19-53C40876125F}" name="key"/>
     <tableColumn id="2" xr3:uid="{8969FEC0-AADF-46CE-8C23-D03ADE795753}" name="en"/>
@@ -3696,15 +3705,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4B28FF-857C-4B73-BD2F-84CA03D2F2FC}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.83203125" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
@@ -3745,33 +3754,33 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>643</v>
+        <v>689</v>
       </c>
       <c r="B2" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="C2" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="I2" t="s">
-        <v>661</v>
+        <v>675</v>
       </c>
       <c r="J2" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="B3" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="C3" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="I3" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="J3" t="s">
         <v>671</v>
@@ -3779,10 +3788,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>645</v>
+        <v>653</v>
       </c>
       <c r="B4" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C4" t="s">
         <v>671</v>
@@ -3796,10 +3805,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>646</v>
+        <v>655</v>
       </c>
       <c r="B5" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C5" t="s">
         <v>671</v>
@@ -3813,41 +3822,41 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="B6" t="s">
-        <v>661</v>
+        <v>667</v>
       </c>
       <c r="C6" t="s">
-        <v>661</v>
+        <v>673</v>
       </c>
       <c r="I6" t="s">
-        <v>661</v>
+        <v>676</v>
       </c>
       <c r="J6" t="s">
-        <v>661</v>
+        <v>673</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>648</v>
+        <v>657</v>
       </c>
       <c r="B7" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="C7" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="I7" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="J7" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>649</v>
+        <v>659</v>
       </c>
       <c r="B8" t="s">
         <v>665</v>
@@ -3864,112 +3873,112 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>650</v>
+        <v>658</v>
       </c>
       <c r="B9" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="C9" t="s">
-        <v>661</v>
+        <v>671</v>
       </c>
       <c r="I9" t="s">
-        <v>661</v>
+        <v>675</v>
       </c>
       <c r="J9" t="s">
-        <v>661</v>
+        <v>671</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>651</v>
+        <v>656</v>
       </c>
       <c r="B10" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="C10" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="I10" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="J10" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="B11" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C11" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="I11" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="J11" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>694</v>
+        <v>644</v>
       </c>
       <c r="B12" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="C12" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="I12" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="J12" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="B13" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C13" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I13" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="J13" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="B14" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="C14" t="s">
-        <v>673</v>
+        <v>661</v>
       </c>
       <c r="I14" t="s">
-        <v>676</v>
+        <v>661</v>
       </c>
       <c r="J14" t="s">
-        <v>673</v>
+        <v>661</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="B15" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C15" t="s">
         <v>671</v>
@@ -3983,104 +3992,121 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="B16" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="C16" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="I16" t="s">
-        <v>676</v>
+        <v>661</v>
       </c>
       <c r="J16" t="s">
-        <v>673</v>
+        <v>661</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>657</v>
+        <v>1025</v>
       </c>
       <c r="B17" t="s">
-        <v>667</v>
+        <v>1026</v>
       </c>
       <c r="C17" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="I17" t="s">
-        <v>676</v>
+        <v>1026</v>
       </c>
       <c r="J17" t="s">
-        <v>673</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="B18" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="C18" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="I18" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="J18" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>659</v>
+        <v>694</v>
       </c>
       <c r="B19" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="C19" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="I19" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="J19" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="B20" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="C20" t="s">
-        <v>673</v>
+        <v>661</v>
       </c>
       <c r="I20" t="s">
-        <v>676</v>
+        <v>661</v>
       </c>
       <c r="J20" t="s">
-        <v>673</v>
+        <v>661</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>689</v>
+        <v>649</v>
       </c>
       <c r="B21" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C21" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I21" t="s">
         <v>675</v>
       </c>
       <c r="J21" t="s">
         <v>671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>660</v>
+      </c>
+      <c r="B22" t="s">
+        <v>668</v>
+      </c>
+      <c r="C22" t="s">
+        <v>673</v>
+      </c>
+      <c r="I22" t="s">
+        <v>676</v>
+      </c>
+      <c r="J22" t="s">
+        <v>673</v>
       </c>
     </row>
   </sheetData>
@@ -4696,7 +4722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5C7B9E-E03D-420F-8955-42B4860CC822}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>